<commit_message>
--logica inicial de alta de usuarios, chequeo de campos repetidos y envio de mail --nuevas traducciones
</commit_message>
<xml_diff>
--- a/Varios/traducciones.xlsx
+++ b/Varios/traducciones.xlsx
@@ -1,31 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Documents\TrabajoDeCampo\trabajo-de-diploma\Varios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Documents\Trabajo-De-Campo\trabajo-de-diploma\Varios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4140C547-61B2-4D95-84BF-FAAB2A18DD79}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBE33DE-AACC-493D-8C64-9BE5EB01BF57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{461B7C5F-BDDA-470F-86DF-9E00192D23ED}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" activeTab="1" xr2:uid="{461B7C5F-BDDA-470F-86DF-9E00192D23ED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Controles" sheetId="1" r:id="rId1"/>
+    <sheet name="Mensajes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="377">
   <si>
     <t>Alumno</t>
   </si>
@@ -171,9 +178,6 @@
     <t>Patentes</t>
   </si>
   <si>
-    <t>Pantentes Incluidas</t>
-  </si>
-  <si>
     <t>Criticidad</t>
   </si>
   <si>
@@ -687,9 +691,6 @@
     <t>com.td.tipo.de.falta</t>
   </si>
   <si>
-    <t>com.td.pantentes.incluidas</t>
-  </si>
-  <si>
     <t>com.td.cambiar.contraseña</t>
   </si>
   <si>
@@ -843,9 +844,6 @@
     <t>Family</t>
   </si>
   <si>
-    <t>Bloqued</t>
-  </si>
-  <si>
     <t>Patent</t>
   </si>
   <si>
@@ -1105,6 +1103,66 @@
   </si>
   <si>
     <t>Fail Course</t>
+  </si>
+  <si>
+    <t>com.td.validacion.alerta</t>
+  </si>
+  <si>
+    <t>com.td.validacion.error</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>com.td.patentes.incluidas</t>
+  </si>
+  <si>
+    <t>Patentes Incluidas</t>
+  </si>
+  <si>
+    <t>Blocked</t>
+  </si>
+  <si>
+    <t>com.td.email.header</t>
+  </si>
+  <si>
+    <t>Su cuenta fue creada con éxito</t>
+  </si>
+  <si>
+    <t>Your account was created successfully</t>
+  </si>
+  <si>
+    <t>com.td.email.body</t>
+  </si>
+  <si>
+    <t>Esta es su contraseña:</t>
+  </si>
+  <si>
+    <t>This is your password:</t>
+  </si>
+  <si>
+    <t>com.td.error.generico</t>
+  </si>
+  <si>
+    <t>Hubo un error al realizar la operación</t>
+  </si>
+  <si>
+    <t>There was an error with the request</t>
+  </si>
+  <si>
+    <t>com.td.completado.generico</t>
+  </si>
+  <si>
+    <t>Su operación fue completada con éxito</t>
+  </si>
+  <si>
+    <t>Your request was completed successfully</t>
+  </si>
+  <si>
+    <t>Campos incompletos o inválidos</t>
+  </si>
+  <si>
+    <t>Incomplete of invalid fields</t>
   </si>
 </sst>
 </file>
@@ -1458,8 +1516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB4AC18-9E40-4F52-A240-1F2EFB37F2BC}">
   <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1473,7 +1531,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
         <v>44</v>
@@ -1482,21 +1540,21 @@
         <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="E1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D65" si="0">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
@@ -1523,13 +1581,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
@@ -1542,13 +1600,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
@@ -1561,13 +1619,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
@@ -1580,13 +1638,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -1599,13 +1657,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
@@ -1618,13 +1676,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
@@ -1637,13 +1695,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
@@ -1656,13 +1714,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -1675,13 +1733,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
@@ -1694,7 +1752,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -1713,13 +1771,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
@@ -1732,13 +1790,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
@@ -1751,13 +1809,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
@@ -1770,13 +1828,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
@@ -1789,13 +1847,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
@@ -1808,13 +1866,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B18" t="s">
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
@@ -1827,13 +1885,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
@@ -1846,13 +1904,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B20" t="s">
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
@@ -1865,13 +1923,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
@@ -1884,13 +1942,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B22" t="s">
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
@@ -1903,13 +1961,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
@@ -1922,13 +1980,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
@@ -1941,13 +1999,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B25" t="s">
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
@@ -1960,13 +2018,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B26" t="s">
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
@@ -1979,13 +2037,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B27" t="s">
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
@@ -1998,13 +2056,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B28" t="s">
         <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
@@ -2017,13 +2075,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B29" t="s">
         <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
@@ -2036,13 +2094,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B30" t="s">
         <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
@@ -2055,13 +2113,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B31" t="s">
         <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
@@ -2074,13 +2132,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B32" t="s">
         <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
@@ -2093,13 +2151,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B33" t="s">
         <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
@@ -2112,13 +2170,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B34" t="s">
         <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
@@ -2131,13 +2189,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B35" t="s">
         <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
@@ -2150,13 +2208,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B36" t="s">
         <v>32</v>
       </c>
       <c r="C36" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
@@ -2169,13 +2227,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B37" t="s">
         <v>33</v>
       </c>
       <c r="C37" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
@@ -2188,13 +2246,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B38" t="s">
         <v>34</v>
       </c>
       <c r="C38" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
@@ -2207,13 +2265,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B39" t="s">
         <v>35</v>
       </c>
       <c r="C39" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
@@ -2226,13 +2284,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B40" t="s">
         <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>272</v>
+        <v>362</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
@@ -2240,18 +2298,18 @@
       </c>
       <c r="E40" t="str">
         <f t="shared" si="1"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.bloqueada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Bloqued')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.bloqueada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Blocked')</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B41" t="s">
         <v>37</v>
       </c>
       <c r="C41" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
@@ -2264,13 +2322,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B42" t="s">
         <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D42" t="str">
         <f t="shared" si="0"/>
@@ -2283,13 +2341,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B43" t="s">
         <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
@@ -2302,13 +2360,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B44" t="s">
         <v>40</v>
       </c>
       <c r="C44" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D44" t="str">
         <f t="shared" si="0"/>
@@ -2321,7 +2379,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B45" t="s">
         <v>41</v>
@@ -2340,7 +2398,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B46" t="s">
         <v>42</v>
@@ -2359,13 +2417,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B47" t="s">
         <v>43</v>
       </c>
       <c r="C47" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="0"/>
@@ -2378,13 +2436,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B48" t="s">
         <v>44</v>
       </c>
       <c r="C48" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D48" t="str">
         <f t="shared" si="0"/>
@@ -2397,13 +2455,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B49" t="s">
         <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="0"/>
@@ -2416,13 +2474,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B50" t="s">
         <v>46</v>
       </c>
       <c r="C50" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
@@ -2435,13 +2493,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B51" t="s">
         <v>47</v>
       </c>
       <c r="C51" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" si="0"/>
@@ -2454,32 +2512,32 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>220</v>
+        <v>360</v>
       </c>
       <c r="B52" t="s">
-        <v>48</v>
+        <v>361</v>
       </c>
       <c r="C52" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D52" t="str">
         <f t="shared" si="0"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.pantentes.incluidas',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Pantentes Incluidas')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.patentes.incluidas',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Patentes Incluidas')</v>
       </c>
       <c r="E52" t="str">
         <f t="shared" si="1"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.pantentes.incluidas',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Included Patents')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.patentes.incluidas',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Included Patents')</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C53" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D53" t="str">
         <f t="shared" si="0"/>
@@ -2492,13 +2550,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C54" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D54" t="str">
         <f t="shared" si="0"/>
@@ -2511,13 +2569,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C55" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D55" t="str">
         <f t="shared" si="0"/>
@@ -2530,13 +2588,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C56" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
@@ -2549,13 +2607,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C57" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D57" t="str">
         <f t="shared" si="0"/>
@@ -2568,13 +2626,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C58" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D58" t="str">
         <f t="shared" si="0"/>
@@ -2587,13 +2645,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C59" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D59" t="str">
         <f t="shared" si="0"/>
@@ -2606,13 +2664,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B60" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C60" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D60" t="str">
         <f t="shared" si="0"/>
@@ -2625,13 +2683,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C61" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
@@ -2644,13 +2702,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B62" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C62" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
@@ -2663,13 +2721,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C63" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
@@ -2682,13 +2740,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B64" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C64" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
@@ -2701,13 +2759,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C65" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
@@ -2720,13 +2778,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B66" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C66" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D66" t="str">
         <f t="shared" ref="D66:D123" si="2">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
@@ -2753,13 +2811,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C67" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D67" t="str">
         <f t="shared" si="2"/>
@@ -2772,13 +2830,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B68" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C68" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D68" t="str">
         <f t="shared" si="2"/>
@@ -2791,13 +2849,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B69" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C69" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D69" t="str">
         <f t="shared" si="2"/>
@@ -2810,13 +2868,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C70" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="2"/>
@@ -2829,13 +2887,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B71" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C71" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D71" t="str">
         <f t="shared" si="2"/>
@@ -2848,13 +2906,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B72" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C72" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D72" t="str">
         <f t="shared" si="2"/>
@@ -2867,13 +2925,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B73" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C73" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="2"/>
@@ -2886,13 +2944,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B74" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C74" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="2"/>
@@ -2905,13 +2963,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B75" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C75" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="2"/>
@@ -2924,13 +2982,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B76" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C76" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D76" t="str">
         <f t="shared" si="2"/>
@@ -2943,13 +3001,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B77" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C77" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="2"/>
@@ -2962,13 +3020,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B78" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C78" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="2"/>
@@ -2981,13 +3039,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B79" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C79" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="2"/>
@@ -3000,13 +3058,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B80" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C80" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D80" t="str">
         <f t="shared" si="2"/>
@@ -3019,13 +3077,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B81" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C81" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D81" t="str">
         <f t="shared" si="2"/>
@@ -3038,13 +3096,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B82" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C82" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="2"/>
@@ -3057,13 +3115,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B83" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C83" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D83" t="str">
         <f t="shared" si="2"/>
@@ -3076,13 +3134,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B84" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C84" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D84" t="str">
         <f t="shared" si="2"/>
@@ -3095,13 +3153,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B85" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C85" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D85" t="str">
         <f t="shared" si="2"/>
@@ -3114,13 +3172,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B86" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C86" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D86" t="str">
         <f t="shared" si="2"/>
@@ -3133,13 +3191,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B87" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C87" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D87" t="str">
         <f t="shared" si="2"/>
@@ -3152,13 +3210,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B88" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C88" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D88" t="str">
         <f t="shared" si="2"/>
@@ -3171,13 +3229,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B89" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C89" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D89" t="str">
         <f t="shared" si="2"/>
@@ -3190,13 +3248,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B90" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C90" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D90" t="str">
         <f t="shared" si="2"/>
@@ -3209,13 +3267,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B91" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C91" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D91" t="str">
         <f t="shared" si="2"/>
@@ -3228,13 +3286,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B92" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C92" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D92" t="str">
         <f t="shared" si="2"/>
@@ -3247,13 +3305,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B93" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C93" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D93" t="str">
         <f t="shared" si="2"/>
@@ -3266,13 +3324,13 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B94" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C94" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D94" t="str">
         <f t="shared" si="2"/>
@@ -3285,13 +3343,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B95" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C95" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D95" t="str">
         <f t="shared" si="2"/>
@@ -3304,13 +3362,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B96" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C96" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D96" t="str">
         <f t="shared" si="2"/>
@@ -3323,13 +3381,13 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B97" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C97" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D97" t="str">
         <f t="shared" si="2"/>
@@ -3342,13 +3400,13 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B98" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C98" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D98" t="str">
         <f t="shared" si="2"/>
@@ -3361,13 +3419,13 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B99" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C99" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D99" t="str">
         <f t="shared" si="2"/>
@@ -3380,13 +3438,13 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B100" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C100" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D100" t="str">
         <f t="shared" si="2"/>
@@ -3399,13 +3457,13 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B101" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C101" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D101" t="str">
         <f t="shared" si="2"/>
@@ -3418,13 +3476,13 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B102" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C102" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D102" t="str">
         <f t="shared" si="2"/>
@@ -3437,13 +3495,13 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B103" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C103" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D103" t="str">
         <f t="shared" si="2"/>
@@ -3456,13 +3514,13 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C104" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D104" t="str">
         <f t="shared" si="2"/>
@@ -3475,13 +3533,13 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B105" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C105" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D105" t="str">
         <f t="shared" si="2"/>
@@ -3494,13 +3552,13 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B106" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C106" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D106" t="str">
         <f t="shared" si="2"/>
@@ -3513,13 +3571,13 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B107" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C107" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D107" t="str">
         <f t="shared" si="2"/>
@@ -3532,13 +3590,13 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B108" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C108" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D108" t="str">
         <f t="shared" si="2"/>
@@ -3551,13 +3609,13 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B109" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C109" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D109" t="str">
         <f t="shared" si="2"/>
@@ -3570,13 +3628,13 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B110" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C110" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D110" t="str">
         <f t="shared" si="2"/>
@@ -3589,13 +3647,13 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B111" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C111" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D111" t="str">
         <f t="shared" si="2"/>
@@ -3608,13 +3666,13 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B112" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C112" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D112" t="str">
         <f t="shared" si="2"/>
@@ -3627,13 +3685,13 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B113" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C113" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D113" t="str">
         <f t="shared" si="2"/>
@@ -3646,13 +3704,13 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B114" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C114" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D114" t="str">
         <f t="shared" si="2"/>
@@ -3665,13 +3723,13 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B115" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C115" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D115" t="str">
         <f t="shared" si="2"/>
@@ -3684,13 +3742,13 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B116" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C116" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D116" t="str">
         <f t="shared" si="2"/>
@@ -3703,13 +3761,13 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B117" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C117" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D117" t="str">
         <f t="shared" si="2"/>
@@ -3722,13 +3780,13 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B118" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C118" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D118" t="str">
         <f t="shared" si="2"/>
@@ -3741,13 +3799,13 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B119" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C119" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D119" t="str">
         <f t="shared" si="2"/>
@@ -3760,13 +3818,13 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B120" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C120" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D120" t="str">
         <f t="shared" si="2"/>
@@ -3779,13 +3837,13 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B121" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C121" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D121" t="str">
         <f t="shared" si="2"/>
@@ -3798,13 +3856,13 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B122" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C122" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D122" t="str">
         <f t="shared" si="2"/>
@@ -3817,13 +3875,13 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B123" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C123" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D123" t="str">
         <f t="shared" si="2"/>
@@ -3836,13 +3894,13 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B124" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C124" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D124" t="str">
         <f>CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
@@ -3871,4 +3929,171 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53349ADF-E49C-4AF5-AC6A-4E299642707C}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="190.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="184.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>344</v>
+      </c>
+      <c r="E1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C2" t="s">
+        <v>376</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D7" si="0">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+values ('",
+$A2,
+"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
+$D$1,
+"'),'",
+$B2,
+"')"))</f>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.validacion.alerta',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Campos incompletos o inválidos')</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E7" si="1">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+values ('",
+$A2,
+"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
+$E$1,
+"'),'",
+$C2,
+"')"))</f>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.validacion.alerta',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Incomplete of invalid fields')</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>358</v>
+      </c>
+      <c r="B3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C3" t="s">
+        <v>359</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.validacion.error',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Error')</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.validacion.error',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Error')</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>363</v>
+      </c>
+      <c r="B4" t="s">
+        <v>364</v>
+      </c>
+      <c r="C4" t="s">
+        <v>365</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.header',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Su cuenta fue creada con éxito')</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.header',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Your account was created successfully')</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>366</v>
+      </c>
+      <c r="B5" t="s">
+        <v>367</v>
+      </c>
+      <c r="C5" t="s">
+        <v>368</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.body',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Esta es su contraseña:')</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.body',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'This is your password:')</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>369</v>
+      </c>
+      <c r="B6" t="s">
+        <v>370</v>
+      </c>
+      <c r="C6" t="s">
+        <v>371</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.error.generico',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Hubo un error al realizar la operación')</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.error.generico',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'There was an error with the request')</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>372</v>
+      </c>
+      <c r="B7" t="s">
+        <v>373</v>
+      </c>
+      <c r="C7" t="s">
+        <v>374</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.completado.generico',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Su operación fue completada con éxito')</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.completado.generico',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Your request was completed successfully')</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
-- fin de usuarios , inicio abm familias
</commit_message>
<xml_diff>
--- a/Varios/traducciones.xlsx
+++ b/Varios/traducciones.xlsx
@@ -1,31 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Documents\Trabajo-De-Campo\trabajo-de-diploma\Varios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Documents\TrabajoDeCampo\trabajo-de-diploma\Varios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBE33DE-AACC-493D-8C64-9BE5EB01BF57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3EFC3164-2DFF-484E-905C-72D37544CD3F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" activeTab="1" xr2:uid="{461B7C5F-BDDA-470F-86DF-9E00192D23ED}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{461B7C5F-BDDA-470F-86DF-9E00192D23ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Controles" sheetId="1" r:id="rId1"/>
     <sheet name="Mensajes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -109,9 +103,6 @@
     <t>Borrar</t>
   </si>
   <si>
-    <t>Modificiar</t>
-  </si>
-  <si>
     <t>Datos</t>
   </si>
   <si>
@@ -1163,6 +1154,9 @@
   </si>
   <si>
     <t>Incomplete of invalid fields</t>
+  </si>
+  <si>
+    <t>Modificar</t>
   </si>
 </sst>
 </file>
@@ -1516,8 +1510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB4AC18-9E40-4F52-A240-1F2EFB37F2BC}">
   <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A125" sqref="A125"/>
+    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,30 +1525,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
-        <v>45</v>
-      </c>
       <c r="D1" t="s">
+        <v>343</v>
+      </c>
+      <c r="E1" t="s">
         <v>344</v>
-      </c>
-      <c r="E1" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D65" si="0">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
@@ -1581,13 +1575,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
@@ -1600,13 +1594,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>345</v>
+      </c>
+      <c r="B4" t="s">
         <v>346</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>347</v>
-      </c>
-      <c r="C4" t="s">
-        <v>348</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
@@ -1619,13 +1613,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
@@ -1638,13 +1632,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -1657,13 +1651,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
@@ -1676,13 +1670,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
@@ -1695,13 +1689,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
@@ -1714,13 +1708,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -1733,13 +1727,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
@@ -1752,7 +1746,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -1771,13 +1765,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
@@ -1790,13 +1784,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
@@ -1809,13 +1803,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
@@ -1828,13 +1822,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
@@ -1847,13 +1841,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
@@ -1866,13 +1860,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B18" t="s">
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
@@ -1885,13 +1879,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
@@ -1904,13 +1898,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B20" t="s">
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
@@ -1923,13 +1917,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
@@ -1942,13 +1936,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B22" t="s">
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
@@ -1961,13 +1955,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
@@ -1980,13 +1974,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
@@ -1999,13 +1993,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B25" t="s">
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
@@ -2018,13 +2012,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B26" t="s">
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
@@ -2037,13 +2031,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B27" t="s">
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
@@ -2056,13 +2050,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B28" t="s">
         <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
@@ -2075,17 +2069,17 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>376</v>
       </c>
       <c r="C29" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.modificar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Modificiar')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.modificar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Modificar')</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="1"/>
@@ -2094,13 +2088,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
@@ -2113,13 +2107,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
@@ -2132,13 +2126,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C32" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
@@ -2151,13 +2145,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
@@ -2170,13 +2164,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C34" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
@@ -2189,13 +2183,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
@@ -2208,13 +2202,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
@@ -2227,13 +2221,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C37" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
@@ -2246,13 +2240,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C38" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
@@ -2265,13 +2259,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C39" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
@@ -2284,13 +2278,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C40" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
@@ -2303,13 +2297,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
@@ -2322,13 +2316,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C42" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D42" t="str">
         <f t="shared" si="0"/>
@@ -2341,13 +2335,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C43" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
@@ -2360,13 +2354,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D44" t="str">
         <f t="shared" si="0"/>
@@ -2379,13 +2373,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="0"/>
@@ -2398,13 +2392,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="0"/>
@@ -2417,13 +2411,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C47" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="0"/>
@@ -2436,13 +2430,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C48" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D48" t="str">
         <f t="shared" si="0"/>
@@ -2455,13 +2449,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C49" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="0"/>
@@ -2474,13 +2468,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
@@ -2493,13 +2487,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" si="0"/>
@@ -2512,13 +2506,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>359</v>
+      </c>
+      <c r="B52" t="s">
         <v>360</v>
       </c>
-      <c r="B52" t="s">
-        <v>361</v>
-      </c>
       <c r="C52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D52" t="str">
         <f t="shared" si="0"/>
@@ -2531,13 +2525,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B53" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C53" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D53" t="str">
         <f t="shared" si="0"/>
@@ -2550,13 +2544,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B54" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C54" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D54" t="str">
         <f t="shared" si="0"/>
@@ -2569,13 +2563,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B55" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C55" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D55" t="str">
         <f t="shared" si="0"/>
@@ -2588,13 +2582,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C56" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
@@ -2607,13 +2601,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B57" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C57" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D57" t="str">
         <f t="shared" si="0"/>
@@ -2626,13 +2620,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B58" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C58" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D58" t="str">
         <f t="shared" si="0"/>
@@ -2645,13 +2639,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B59" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C59" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D59" t="str">
         <f t="shared" si="0"/>
@@ -2664,13 +2658,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B60" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C60" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D60" t="str">
         <f t="shared" si="0"/>
@@ -2683,13 +2677,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B61" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C61" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
@@ -2702,13 +2696,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C62" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
@@ -2721,13 +2715,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B63" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C63" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
@@ -2740,13 +2734,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C64" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
@@ -2759,13 +2753,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B65" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C65" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
@@ -2778,13 +2772,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C66" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D66" t="str">
         <f t="shared" ref="D66:D123" si="2">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
@@ -2811,13 +2805,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B67" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C67" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D67" t="str">
         <f t="shared" si="2"/>
@@ -2830,13 +2824,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B68" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C68" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D68" t="str">
         <f t="shared" si="2"/>
@@ -2849,13 +2843,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B69" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C69" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D69" t="str">
         <f t="shared" si="2"/>
@@ -2868,13 +2862,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B70" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C70" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="2"/>
@@ -2887,13 +2881,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B71" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C71" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D71" t="str">
         <f t="shared" si="2"/>
@@ -2906,13 +2900,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B72" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C72" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D72" t="str">
         <f t="shared" si="2"/>
@@ -2925,13 +2919,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B73" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C73" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="2"/>
@@ -2944,13 +2938,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C74" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="2"/>
@@ -2963,13 +2957,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B75" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C75" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="2"/>
@@ -2982,13 +2976,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B76" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C76" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D76" t="str">
         <f t="shared" si="2"/>
@@ -3001,13 +2995,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B77" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C77" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="2"/>
@@ -3020,13 +3014,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B78" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C78" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="2"/>
@@ -3039,13 +3033,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B79" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C79" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="2"/>
@@ -3058,13 +3052,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B80" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C80" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D80" t="str">
         <f t="shared" si="2"/>
@@ -3077,13 +3071,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B81" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C81" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D81" t="str">
         <f t="shared" si="2"/>
@@ -3096,13 +3090,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B82" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C82" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="2"/>
@@ -3115,13 +3109,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B83" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C83" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D83" t="str">
         <f t="shared" si="2"/>
@@ -3134,13 +3128,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B84" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C84" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D84" t="str">
         <f t="shared" si="2"/>
@@ -3153,13 +3147,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B85" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C85" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D85" t="str">
         <f t="shared" si="2"/>
@@ -3172,13 +3166,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B86" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C86" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D86" t="str">
         <f t="shared" si="2"/>
@@ -3191,13 +3185,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B87" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C87" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D87" t="str">
         <f t="shared" si="2"/>
@@ -3210,13 +3204,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B88" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C88" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D88" t="str">
         <f t="shared" si="2"/>
@@ -3229,13 +3223,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B89" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C89" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D89" t="str">
         <f t="shared" si="2"/>
@@ -3248,13 +3242,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B90" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C90" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D90" t="str">
         <f t="shared" si="2"/>
@@ -3267,13 +3261,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B91" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C91" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D91" t="str">
         <f t="shared" si="2"/>
@@ -3286,13 +3280,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B92" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C92" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D92" t="str">
         <f t="shared" si="2"/>
@@ -3305,13 +3299,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B93" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C93" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D93" t="str">
         <f t="shared" si="2"/>
@@ -3324,13 +3318,13 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B94" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C94" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D94" t="str">
         <f t="shared" si="2"/>
@@ -3343,13 +3337,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B95" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C95" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D95" t="str">
         <f t="shared" si="2"/>
@@ -3362,13 +3356,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B96" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C96" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D96" t="str">
         <f t="shared" si="2"/>
@@ -3381,13 +3375,13 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B97" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C97" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D97" t="str">
         <f t="shared" si="2"/>
@@ -3400,13 +3394,13 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B98" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C98" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D98" t="str">
         <f t="shared" si="2"/>
@@ -3419,13 +3413,13 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B99" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C99" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D99" t="str">
         <f t="shared" si="2"/>
@@ -3438,13 +3432,13 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B100" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C100" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D100" t="str">
         <f t="shared" si="2"/>
@@ -3457,13 +3451,13 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B101" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C101" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D101" t="str">
         <f t="shared" si="2"/>
@@ -3476,13 +3470,13 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B102" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C102" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D102" t="str">
         <f t="shared" si="2"/>
@@ -3495,13 +3489,13 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B103" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C103" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D103" t="str">
         <f t="shared" si="2"/>
@@ -3514,13 +3508,13 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B104" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C104" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D104" t="str">
         <f t="shared" si="2"/>
@@ -3533,13 +3527,13 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B105" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C105" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D105" t="str">
         <f t="shared" si="2"/>
@@ -3552,13 +3546,13 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B106" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C106" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D106" t="str">
         <f t="shared" si="2"/>
@@ -3571,13 +3565,13 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B107" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C107" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D107" t="str">
         <f t="shared" si="2"/>
@@ -3590,13 +3584,13 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B108" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C108" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D108" t="str">
         <f t="shared" si="2"/>
@@ -3609,13 +3603,13 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B109" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C109" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D109" t="str">
         <f t="shared" si="2"/>
@@ -3628,13 +3622,13 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B110" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C110" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D110" t="str">
         <f t="shared" si="2"/>
@@ -3647,13 +3641,13 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B111" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C111" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D111" t="str">
         <f t="shared" si="2"/>
@@ -3666,13 +3660,13 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B112" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C112" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D112" t="str">
         <f t="shared" si="2"/>
@@ -3685,13 +3679,13 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B113" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C113" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D113" t="str">
         <f t="shared" si="2"/>
@@ -3704,13 +3698,13 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B114" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C114" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D114" t="str">
         <f t="shared" si="2"/>
@@ -3723,13 +3717,13 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B115" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C115" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D115" t="str">
         <f t="shared" si="2"/>
@@ -3742,13 +3736,13 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B116" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C116" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D116" t="str">
         <f t="shared" si="2"/>
@@ -3761,13 +3755,13 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B117" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C117" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D117" t="str">
         <f t="shared" si="2"/>
@@ -3780,13 +3774,13 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B118" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C118" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D118" t="str">
         <f t="shared" si="2"/>
@@ -3799,13 +3793,13 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B119" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C119" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D119" t="str">
         <f t="shared" si="2"/>
@@ -3818,13 +3812,13 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B120" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C120" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D120" t="str">
         <f t="shared" si="2"/>
@@ -3837,13 +3831,13 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B121" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C121" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D121" t="str">
         <f t="shared" si="2"/>
@@ -3856,13 +3850,13 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
+        <v>348</v>
+      </c>
+      <c r="B122" t="s">
         <v>349</v>
       </c>
-      <c r="B122" t="s">
+      <c r="C122" t="s">
         <v>350</v>
-      </c>
-      <c r="C122" t="s">
-        <v>351</v>
       </c>
       <c r="D122" t="str">
         <f t="shared" si="2"/>
@@ -3875,13 +3869,13 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B123" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C123" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D123" t="str">
         <f t="shared" si="2"/>
@@ -3894,13 +3888,13 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
+        <v>353</v>
+      </c>
+      <c r="B124" t="s">
         <v>354</v>
       </c>
-      <c r="B124" t="s">
+      <c r="C124" t="s">
         <v>355</v>
-      </c>
-      <c r="C124" t="s">
-        <v>356</v>
       </c>
       <c r="D124" t="str">
         <f>CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
@@ -3935,8 +3929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53349ADF-E49C-4AF5-AC6A-4E299642707C}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3950,30 +3944,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
-        <v>45</v>
-      </c>
       <c r="D1" t="s">
+        <v>343</v>
+      </c>
+      <c r="E1" t="s">
         <v>344</v>
-      </c>
-      <c r="E1" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C2" t="s">
         <v>375</v>
-      </c>
-      <c r="C2" t="s">
-        <v>376</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D7" si="0">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
@@ -4000,13 +3994,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>357</v>
+      </c>
+      <c r="B3" t="s">
         <v>358</v>
       </c>
-      <c r="B3" t="s">
-        <v>359</v>
-      </c>
       <c r="C3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
@@ -4019,13 +4013,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>362</v>
+      </c>
+      <c r="B4" t="s">
         <v>363</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>364</v>
-      </c>
-      <c r="C4" t="s">
-        <v>365</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
@@ -4038,13 +4032,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>365</v>
+      </c>
+      <c r="B5" t="s">
         <v>366</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>367</v>
-      </c>
-      <c r="C5" t="s">
-        <v>368</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
@@ -4057,13 +4051,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>368</v>
+      </c>
+      <c r="B6" t="s">
         <v>369</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>370</v>
-      </c>
-      <c r="C6" t="s">
-        <v>371</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -4076,13 +4070,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>371</v>
+      </c>
+      <c r="B7" t="s">
         <v>372</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>373</v>
-      </c>
-      <c r="C7" t="s">
-        <v>374</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
-translations cross app -fin reportes -bloqueo de botones basado enpermisos
</commit_message>
<xml_diff>
--- a/Varios/traducciones.xlsx
+++ b/Varios/traducciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Documents\TrabajoDeCampo\trabajo-de-diploma\Varios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Documents\Trabajo-De-Campo\trabajo-de-diploma\Varios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3EFC3164-2DFF-484E-905C-72D37544CD3F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3709192C-1B55-4266-937E-7A172A77A702}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{461B7C5F-BDDA-470F-86DF-9E00192D23ED}"/>
   </bookViews>
@@ -16,17 +16,23 @@
     <sheet name="Controles" sheetId="1" r:id="rId1"/>
     <sheet name="Mensajes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="491">
   <si>
     <t>Alumno</t>
   </si>
@@ -913,9 +919,6 @@
     <t>Assigned Patents</t>
   </si>
   <si>
-    <t>Databasa backup</t>
-  </si>
-  <si>
     <t>Select destination</t>
   </si>
   <si>
@@ -1157,14 +1160,367 @@
   </si>
   <si>
     <t>Modificar</t>
+  </si>
+  <si>
+    <t>com.td.valor</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>com.td.motivo</t>
+  </si>
+  <si>
+    <t>Motivo</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>com.td.crear</t>
+  </si>
+  <si>
+    <t>Crear</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>com.td.niveles</t>
+  </si>
+  <si>
+    <t>Levels</t>
+  </si>
+  <si>
+    <t>Niveles</t>
+  </si>
+  <si>
+    <t>com.td.tipo</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>com.td.egresar</t>
+  </si>
+  <si>
+    <t>Egresar</t>
+  </si>
+  <si>
+    <t>Graduate</t>
+  </si>
+  <si>
+    <t>Promocionar</t>
+  </si>
+  <si>
+    <t>Promote</t>
+  </si>
+  <si>
+    <t>com.td.bloqueado</t>
+  </si>
+  <si>
+    <t>Bloqueado</t>
+  </si>
+  <si>
+    <t>com.td.si</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>com.td.no</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Database backup</t>
+  </si>
+  <si>
+    <t>Generar Respaldo</t>
+  </si>
+  <si>
+    <t>Generate Backup</t>
+  </si>
+  <si>
+    <t>com.td.generate.respaldo</t>
+  </si>
+  <si>
+    <t>com.td.contiene</t>
+  </si>
+  <si>
+    <t>Contiene</t>
+  </si>
+  <si>
+    <t>Contains</t>
+  </si>
+  <si>
+    <t>com.td.criticidad.alta</t>
+  </si>
+  <si>
+    <t>com.td.criticidad.media</t>
+  </si>
+  <si>
+    <t>com.td.criticidad.baja</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Baja</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>com.td.menu</t>
+  </si>
+  <si>
+    <t>Gestión Educativa</t>
+  </si>
+  <si>
+    <t>Education Management</t>
+  </si>
+  <si>
+    <t>Tutor</t>
+  </si>
+  <si>
+    <t>com.td.tutor</t>
+  </si>
+  <si>
+    <t>com.td.faltas.totales</t>
+  </si>
+  <si>
+    <t>Faltas Totales</t>
+  </si>
+  <si>
+    <t>Total Abscences</t>
+  </si>
+  <si>
+    <t>com.td.disclaimer</t>
+  </si>
+  <si>
+    <t>The courses marked with red are exceeded</t>
+  </si>
+  <si>
+    <t>Los cursos marcados en rojo se estan excedidos</t>
+  </si>
+  <si>
+    <t>com.td.maximo</t>
+  </si>
+  <si>
+    <t>Máximo</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>com.td.actual</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>com.td.plan.estudios</t>
+  </si>
+  <si>
+    <t>Plan de estudios</t>
+  </si>
+  <si>
+    <t>Curriculum</t>
+  </si>
+  <si>
+    <t>com.td.complete.campos</t>
+  </si>
+  <si>
+    <t>com.td.completado</t>
+  </si>
+  <si>
+    <t>Completado</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>com.td.existe.materia</t>
+  </si>
+  <si>
+    <t>Ya existe la materia</t>
+  </si>
+  <si>
+    <t>The class already exists</t>
+  </si>
+  <si>
+    <t>com.td.descartar</t>
+  </si>
+  <si>
+    <t>Descartar cambios</t>
+  </si>
+  <si>
+    <t>DiscardChanges</t>
+  </si>
+  <si>
+    <t>com.td.seleccione.horario</t>
+  </si>
+  <si>
+    <t>Seleccione un horario</t>
+  </si>
+  <si>
+    <t>Select a schedule</t>
+  </si>
+  <si>
+    <t>com.td.falta.horario</t>
+  </si>
+  <si>
+    <t>There is no schedule there</t>
+  </si>
+  <si>
+    <t>No hay un horario ahí</t>
+  </si>
+  <si>
+    <t>com.td.materia.asignada</t>
+  </si>
+  <si>
+    <t>La materia esta asignada</t>
+  </si>
+  <si>
+    <t>The class is assigned</t>
+  </si>
+  <si>
+    <t>com.td.seleccione.busqueda</t>
+  </si>
+  <si>
+    <t>Seleccione datos de busqueda</t>
+  </si>
+  <si>
+    <t>Select something to search by</t>
+  </si>
+  <si>
+    <t>Complete all the required fields</t>
+  </si>
+  <si>
+    <t>com.td.orientacion.incorrecta</t>
+  </si>
+  <si>
+    <t>La orientacion no corresponde al curso</t>
+  </si>
+  <si>
+    <t>The course does not have that orientation</t>
+  </si>
+  <si>
+    <t>com.td.tutor.requerido</t>
+  </si>
+  <si>
+    <t>Se requiere al menos un tutor</t>
+  </si>
+  <si>
+    <t>At least one tutor required</t>
+  </si>
+  <si>
+    <t>com.td.dni.repetido</t>
+  </si>
+  <si>
+    <t>D.N.I. ya existente</t>
+  </si>
+  <si>
+    <t>ID already exists</t>
+  </si>
+  <si>
+    <t>com.td.fecha.ocupada</t>
+  </si>
+  <si>
+    <t>Fecha ocupada</t>
+  </si>
+  <si>
+    <t>Date already entered</t>
+  </si>
+  <si>
+    <t>com.td.char.count</t>
+  </si>
+  <si>
+    <t>Como mínimo 8 caracteres</t>
+  </si>
+  <si>
+    <t>At least 8 characters</t>
+  </si>
+  <si>
+    <t>com.td.pass.iguales</t>
+  </si>
+  <si>
+    <t>Las contraseñas son iguales</t>
+  </si>
+  <si>
+    <t>The passwords are the same one</t>
+  </si>
+  <si>
+    <t>com.td.pass.no.coinciden</t>
+  </si>
+  <si>
+    <t>Las contraseñas son no coinciden</t>
+  </si>
+  <si>
+    <t>The passwords don´t match</t>
+  </si>
+  <si>
+    <t>Complete todos los campos requeridos</t>
+  </si>
+  <si>
+    <t>com.td.permisos.esenciales</t>
+  </si>
+  <si>
+    <t>Se perderian permisos esenciales</t>
+  </si>
+  <si>
+    <t>Essential roles would be lost</t>
+  </si>
+  <si>
+    <t>com.td.path</t>
+  </si>
+  <si>
+    <t>Seleccione una ruta</t>
+  </si>
+  <si>
+    <t>Select a path</t>
+  </si>
+  <si>
+    <t>com.td.mail.invalido</t>
+  </si>
+  <si>
+    <t>Mail inválido</t>
+  </si>
+  <si>
+    <t>Invalid mail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1192,8 +1548,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1508,10 +1867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB4AC18-9E40-4F52-A240-1F2EFB37F2BC}">
-  <dimension ref="A1:E124"/>
+  <dimension ref="A1:E270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="E131" workbookViewId="0">
+      <selection activeCell="D148" sqref="D148:E165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1534,10 +1893,10 @@
         <v>44</v>
       </c>
       <c r="D1" t="s">
+        <v>342</v>
+      </c>
+      <c r="E1" t="s">
         <v>343</v>
-      </c>
-      <c r="E1" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1594,13 +1953,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>344</v>
+      </c>
+      <c r="B4" t="s">
         <v>345</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>346</v>
-      </c>
-      <c r="C4" t="s">
-        <v>347</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
@@ -2069,10 +2428,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B29" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C29" t="s">
         <v>258</v>
@@ -2284,7 +2643,7 @@
         <v>35</v>
       </c>
       <c r="C40" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
@@ -2506,10 +2865,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>358</v>
+      </c>
+      <c r="B52" t="s">
         <v>359</v>
-      </c>
-      <c r="B52" t="s">
-        <v>360</v>
       </c>
       <c r="C52" t="s">
         <v>276</v>
@@ -2887,7 +3246,7 @@
         <v>65</v>
       </c>
       <c r="C71" t="s">
-        <v>295</v>
+        <v>403</v>
       </c>
       <c r="D71" t="str">
         <f t="shared" si="2"/>
@@ -2895,7 +3254,7 @@
       </c>
       <c r="E71" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.respaldo.base.de.datos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Databasa backup')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.respaldo.base.de.datos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Database backup')</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2925,7 +3284,7 @@
         <v>67</v>
       </c>
       <c r="C73" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="2"/>
@@ -2944,7 +3303,7 @@
         <v>68</v>
       </c>
       <c r="C74" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="2"/>
@@ -2963,7 +3322,7 @@
         <v>69</v>
       </c>
       <c r="C75" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="2"/>
@@ -3001,7 +3360,7 @@
         <v>71</v>
       </c>
       <c r="C77" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="2"/>
@@ -3020,7 +3379,7 @@
         <v>72</v>
       </c>
       <c r="C78" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="2"/>
@@ -3039,7 +3398,7 @@
         <v>73</v>
       </c>
       <c r="C79" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="2"/>
@@ -3058,7 +3417,7 @@
         <v>74</v>
       </c>
       <c r="C80" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D80" t="str">
         <f t="shared" si="2"/>
@@ -3077,7 +3436,7 @@
         <v>75</v>
       </c>
       <c r="C81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D81" t="str">
         <f t="shared" si="2"/>
@@ -3096,7 +3455,7 @@
         <v>76</v>
       </c>
       <c r="C82" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="2"/>
@@ -3115,7 +3474,7 @@
         <v>77</v>
       </c>
       <c r="C83" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D83" t="str">
         <f t="shared" si="2"/>
@@ -3134,7 +3493,7 @@
         <v>78</v>
       </c>
       <c r="C84" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D84" t="str">
         <f t="shared" si="2"/>
@@ -3153,7 +3512,7 @@
         <v>79</v>
       </c>
       <c r="C85" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D85" t="str">
         <f t="shared" si="2"/>
@@ -3191,7 +3550,7 @@
         <v>81</v>
       </c>
       <c r="C87" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D87" t="str">
         <f t="shared" si="2"/>
@@ -3210,7 +3569,7 @@
         <v>82</v>
       </c>
       <c r="C88" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D88" t="str">
         <f t="shared" si="2"/>
@@ -3229,7 +3588,7 @@
         <v>83</v>
       </c>
       <c r="C89" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D89" t="str">
         <f t="shared" si="2"/>
@@ -3248,7 +3607,7 @@
         <v>84</v>
       </c>
       <c r="C90" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D90" t="str">
         <f t="shared" si="2"/>
@@ -3267,7 +3626,7 @@
         <v>85</v>
       </c>
       <c r="C91" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D91" t="str">
         <f t="shared" si="2"/>
@@ -3286,7 +3645,7 @@
         <v>86</v>
       </c>
       <c r="C92" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D92" t="str">
         <f t="shared" si="2"/>
@@ -3305,7 +3664,7 @@
         <v>87</v>
       </c>
       <c r="C93" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D93" t="str">
         <f t="shared" si="2"/>
@@ -3324,7 +3683,7 @@
         <v>88</v>
       </c>
       <c r="C94" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D94" t="str">
         <f t="shared" si="2"/>
@@ -3343,7 +3702,7 @@
         <v>89</v>
       </c>
       <c r="C95" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D95" t="str">
         <f t="shared" si="2"/>
@@ -3362,7 +3721,7 @@
         <v>90</v>
       </c>
       <c r="C96" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D96" t="str">
         <f t="shared" si="2"/>
@@ -3381,7 +3740,7 @@
         <v>91</v>
       </c>
       <c r="C97" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D97" t="str">
         <f t="shared" si="2"/>
@@ -3400,7 +3759,7 @@
         <v>92</v>
       </c>
       <c r="C98" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D98" t="str">
         <f t="shared" si="2"/>
@@ -3419,7 +3778,7 @@
         <v>93</v>
       </c>
       <c r="C99" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D99" t="str">
         <f t="shared" si="2"/>
@@ -3438,7 +3797,7 @@
         <v>94</v>
       </c>
       <c r="C100" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D100" t="str">
         <f t="shared" si="2"/>
@@ -3457,7 +3816,7 @@
         <v>95</v>
       </c>
       <c r="C101" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D101" t="str">
         <f t="shared" si="2"/>
@@ -3476,7 +3835,7 @@
         <v>96</v>
       </c>
       <c r="C102" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D102" t="str">
         <f t="shared" si="2"/>
@@ -3495,7 +3854,7 @@
         <v>97</v>
       </c>
       <c r="C103" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D103" t="str">
         <f t="shared" si="2"/>
@@ -3514,7 +3873,7 @@
         <v>98</v>
       </c>
       <c r="C104" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D104" t="str">
         <f t="shared" si="2"/>
@@ -3533,7 +3892,7 @@
         <v>99</v>
       </c>
       <c r="C105" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D105" t="str">
         <f t="shared" si="2"/>
@@ -3571,7 +3930,7 @@
         <v>101</v>
       </c>
       <c r="C107" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D107" t="str">
         <f t="shared" si="2"/>
@@ -3587,10 +3946,10 @@
         <v>197</v>
       </c>
       <c r="B108" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C108" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D108" t="str">
         <f t="shared" si="2"/>
@@ -3609,7 +3968,7 @@
         <v>102</v>
       </c>
       <c r="C109" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D109" t="str">
         <f t="shared" si="2"/>
@@ -3628,7 +3987,7 @@
         <v>103</v>
       </c>
       <c r="C110" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D110" t="str">
         <f t="shared" si="2"/>
@@ -3647,7 +4006,7 @@
         <v>104</v>
       </c>
       <c r="C111" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D111" t="str">
         <f t="shared" si="2"/>
@@ -3666,7 +4025,7 @@
         <v>105</v>
       </c>
       <c r="C112" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D112" t="str">
         <f t="shared" si="2"/>
@@ -3685,7 +4044,7 @@
         <v>106</v>
       </c>
       <c r="C113" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D113" t="str">
         <f t="shared" si="2"/>
@@ -3704,7 +4063,7 @@
         <v>107</v>
       </c>
       <c r="C114" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D114" t="str">
         <f t="shared" si="2"/>
@@ -3723,7 +4082,7 @@
         <v>108</v>
       </c>
       <c r="C115" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D115" t="str">
         <f t="shared" si="2"/>
@@ -3742,7 +4101,7 @@
         <v>109</v>
       </c>
       <c r="C116" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D116" t="str">
         <f t="shared" si="2"/>
@@ -3761,7 +4120,7 @@
         <v>110</v>
       </c>
       <c r="C117" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D117" t="str">
         <f t="shared" si="2"/>
@@ -3780,7 +4139,7 @@
         <v>111</v>
       </c>
       <c r="C118" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D118" t="str">
         <f t="shared" si="2"/>
@@ -3799,7 +4158,7 @@
         <v>112</v>
       </c>
       <c r="C119" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D119" t="str">
         <f t="shared" si="2"/>
@@ -3818,7 +4177,7 @@
         <v>113</v>
       </c>
       <c r="C120" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D120" t="str">
         <f t="shared" si="2"/>
@@ -3837,7 +4196,7 @@
         <v>114</v>
       </c>
       <c r="C121" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D121" t="str">
         <f t="shared" si="2"/>
@@ -3850,13 +4209,13 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
+        <v>347</v>
+      </c>
+      <c r="B122" t="s">
         <v>348</v>
       </c>
-      <c r="B122" t="s">
+      <c r="C122" t="s">
         <v>349</v>
-      </c>
-      <c r="C122" t="s">
-        <v>350</v>
       </c>
       <c r="D122" t="str">
         <f t="shared" si="2"/>
@@ -3869,13 +4228,13 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B123" t="s">
         <v>94</v>
       </c>
       <c r="C123" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D123" t="str">
         <f t="shared" si="2"/>
@@ -3888,13 +4247,13 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
+        <v>352</v>
+      </c>
+      <c r="B124" t="s">
         <v>353</v>
       </c>
-      <c r="B124" t="s">
+      <c r="C124" t="s">
         <v>354</v>
-      </c>
-      <c r="C124" t="s">
-        <v>355</v>
       </c>
       <c r="D124" t="str">
         <f>CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
@@ -3917,6 +4276,1906 @@
 $C124,
 "')"))</f>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.repetir',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Fail Course')</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B125" t="s">
+        <v>9</v>
+      </c>
+      <c r="C125" t="s">
+        <v>243</v>
+      </c>
+      <c r="D125" t="str">
+        <f>CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+values ('",
+$A125,
+"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
+$D$1,
+"'),'",
+$B125,
+"')"))</f>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.asignado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Asignado')</v>
+      </c>
+      <c r="E125" t="str">
+        <f>CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+values ('",
+$A125,
+"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
+$E$1,
+"'),'",
+$C125,
+"')"))</f>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.asignado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Assigned')</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>376</v>
+      </c>
+      <c r="B126" t="s">
+        <v>377</v>
+      </c>
+      <c r="C126" t="s">
+        <v>378</v>
+      </c>
+      <c r="D126" t="str">
+        <f>CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+values ('",
+$A126,
+"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
+$D$1,
+"'),'",
+$B126,
+"')"))</f>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.valor',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Valor')</v>
+      </c>
+      <c r="E126" t="str">
+        <f>CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+values ('",
+$A126,
+"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
+$E$1,
+"'),'",
+$C126,
+"')"))</f>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.valor',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Value')</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B127" t="s">
+        <v>380</v>
+      </c>
+      <c r="C127" t="s">
+        <v>381</v>
+      </c>
+      <c r="D127" t="str">
+        <f t="shared" ref="D127:D189" si="4">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+values ('",
+$A127,
+"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
+$D$1,
+"'),'",
+$B127,
+"')"))</f>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.motivo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Motivo')</v>
+      </c>
+      <c r="E127" t="str">
+        <f t="shared" ref="E127:E189" si="5">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+values ('",
+$A127,
+"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
+$E$1,
+"'),'",
+$C127,
+"')"))</f>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.motivo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Reason')</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>382</v>
+      </c>
+      <c r="B128" t="s">
+        <v>383</v>
+      </c>
+      <c r="C128" t="s">
+        <v>384</v>
+      </c>
+      <c r="D128" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.crear',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Crear')</v>
+      </c>
+      <c r="E128" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.crear',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Create')</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>385</v>
+      </c>
+      <c r="B129" t="s">
+        <v>387</v>
+      </c>
+      <c r="C129" t="s">
+        <v>386</v>
+      </c>
+      <c r="D129" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.niveles',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Niveles')</v>
+      </c>
+      <c r="E129" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.niveles',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Levels')</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>388</v>
+      </c>
+      <c r="B130" t="s">
+        <v>389</v>
+      </c>
+      <c r="C130" t="s">
+        <v>390</v>
+      </c>
+      <c r="D130" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tipo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Tipo')</v>
+      </c>
+      <c r="E130" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tipo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Type')</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>391</v>
+      </c>
+      <c r="B131" t="s">
+        <v>392</v>
+      </c>
+      <c r="C131" t="s">
+        <v>393</v>
+      </c>
+      <c r="D131" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.egresar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Egresar')</v>
+      </c>
+      <c r="E131" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.egresar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Graduate')</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>207</v>
+      </c>
+      <c r="B132" t="s">
+        <v>394</v>
+      </c>
+      <c r="C132" t="s">
+        <v>395</v>
+      </c>
+      <c r="D132" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.promocionar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Promocionar')</v>
+      </c>
+      <c r="E132" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.promocionar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Promote')</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B133" t="s">
+        <v>397</v>
+      </c>
+      <c r="C133" t="s">
+        <v>360</v>
+      </c>
+      <c r="D133" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.bloqueado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Bloqueado')</v>
+      </c>
+      <c r="E133" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.bloqueado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Blocked')</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B134" t="s">
+        <v>399</v>
+      </c>
+      <c r="C134" t="s">
+        <v>400</v>
+      </c>
+      <c r="D134" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.si',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Sí')</v>
+      </c>
+      <c r="E134" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.si',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Yes')</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B135" t="s">
+        <v>402</v>
+      </c>
+      <c r="C135" t="s">
+        <v>402</v>
+      </c>
+      <c r="D135" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.no',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'No')</v>
+      </c>
+      <c r="E135" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.no',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'No')</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="C136" t="s">
+        <v>405</v>
+      </c>
+      <c r="D136" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.generate.respaldo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Generar Respaldo')</v>
+      </c>
+      <c r="E136" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.generate.respaldo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Generate Backup')</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="C137" t="s">
+        <v>409</v>
+      </c>
+      <c r="D137" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.contiene',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Contiene')</v>
+      </c>
+      <c r="E137" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.contiene',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Contains')</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="C138" t="s">
+        <v>415</v>
+      </c>
+      <c r="D138" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.alta',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Alta')</v>
+      </c>
+      <c r="E138" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.alta',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'High')</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C139" t="s">
+        <v>416</v>
+      </c>
+      <c r="D139" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.media',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Media')</v>
+      </c>
+      <c r="E139" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.media',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Medium')</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="C140" t="s">
+        <v>417</v>
+      </c>
+      <c r="D140" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.baja',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Baja')</v>
+      </c>
+      <c r="E140" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.baja',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Low')</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="C141" t="s">
+        <v>420</v>
+      </c>
+      <c r="D141" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.menu',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Gestión Educativa')</v>
+      </c>
+      <c r="E141" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.menu',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Education Management')</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>422</v>
+      </c>
+      <c r="B142" t="s">
+        <v>421</v>
+      </c>
+      <c r="C142" t="s">
+        <v>421</v>
+      </c>
+      <c r="D142" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Tutor')</v>
+      </c>
+      <c r="E142" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Tutor')</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>423</v>
+      </c>
+      <c r="B143" t="s">
+        <v>424</v>
+      </c>
+      <c r="C143" t="s">
+        <v>425</v>
+      </c>
+      <c r="D143" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.faltas.totales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Faltas Totales')</v>
+      </c>
+      <c r="E143" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.faltas.totales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Total Abscences')</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>426</v>
+      </c>
+      <c r="B144" t="s">
+        <v>428</v>
+      </c>
+      <c r="C144" t="s">
+        <v>427</v>
+      </c>
+      <c r="D144" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.disclaimer',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Los cursos marcados en rojo se estan excedidos')</v>
+      </c>
+      <c r="E144" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.disclaimer',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The courses marked with red are exceeded')</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>429</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="C145" t="s">
+        <v>431</v>
+      </c>
+      <c r="D145" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.maximo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Máximo')</v>
+      </c>
+      <c r="E145" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.maximo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Maximum')</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>432</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="C146" t="s">
+        <v>433</v>
+      </c>
+      <c r="D146" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.actual',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Actual')</v>
+      </c>
+      <c r="E146" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.actual',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Actual')</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>434</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="C147" t="s">
+        <v>436</v>
+      </c>
+      <c r="D147" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.plan.estudios',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Plan de estudios')</v>
+      </c>
+      <c r="E147" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.plan.estudios',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Curriculum')</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>437</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="C148" t="s">
+        <v>459</v>
+      </c>
+      <c r="D148" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.complete.campos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Complete todos los campos requeridos')</v>
+      </c>
+      <c r="E148" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.complete.campos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Complete all the required fields')</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>438</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="C149" t="s">
+        <v>440</v>
+      </c>
+      <c r="D149" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.completado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Completado')</v>
+      </c>
+      <c r="E149" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.completado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Completed')</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>441</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="C150" t="s">
+        <v>443</v>
+      </c>
+      <c r="D150" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.existe.materia',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Ya existe la materia')</v>
+      </c>
+      <c r="E150" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.existe.materia',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The class already exists')</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>444</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="C151" t="s">
+        <v>446</v>
+      </c>
+      <c r="D151" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.descartar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Descartar cambios')</v>
+      </c>
+      <c r="E151" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.descartar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'DiscardChanges')</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>447</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="C152" t="s">
+        <v>449</v>
+      </c>
+      <c r="D152" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seleccione.horario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Seleccione un horario')</v>
+      </c>
+      <c r="E152" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seleccione.horario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Select a schedule')</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>450</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C153" t="s">
+        <v>451</v>
+      </c>
+      <c r="D153" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.falta.horario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'No hay un horario ahí')</v>
+      </c>
+      <c r="E153" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.falta.horario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'There is no schedule there')</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>453</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="C154" t="s">
+        <v>455</v>
+      </c>
+      <c r="D154" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.materia.asignada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'La materia esta asignada')</v>
+      </c>
+      <c r="E154" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.materia.asignada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The class is assigned')</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>456</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="C155" t="s">
+        <v>458</v>
+      </c>
+      <c r="D155" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seleccione.busqueda',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Seleccione datos de busqueda')</v>
+      </c>
+      <c r="E155" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seleccione.busqueda',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Select something to search by')</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>460</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="C156" t="s">
+        <v>462</v>
+      </c>
+      <c r="D156" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.orientacion.incorrecta',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'La orientacion no corresponde al curso')</v>
+      </c>
+      <c r="E156" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.orientacion.incorrecta',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The course does not have that orientation')</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>463</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="C157" t="s">
+        <v>465</v>
+      </c>
+      <c r="D157" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor.requerido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Se requiere al menos un tutor')</v>
+      </c>
+      <c r="E157" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor.requerido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'At least one tutor required')</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>466</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="C158" t="s">
+        <v>468</v>
+      </c>
+      <c r="D158" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.dni.repetido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'D.N.I. ya existente')</v>
+      </c>
+      <c r="E158" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.dni.repetido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'ID already exists')</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>469</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="C159" t="s">
+        <v>471</v>
+      </c>
+      <c r="D159" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.fecha.ocupada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Fecha ocupada')</v>
+      </c>
+      <c r="E159" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.fecha.ocupada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Date already entered')</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>472</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="C160" t="s">
+        <v>474</v>
+      </c>
+      <c r="D160" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.char.count',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Como mínimo 8 caracteres')</v>
+      </c>
+      <c r="E160" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.char.count',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'At least 8 characters')</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>475</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="C161" t="s">
+        <v>477</v>
+      </c>
+      <c r="D161" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.pass.iguales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Las contraseñas son iguales')</v>
+      </c>
+      <c r="E161" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.pass.iguales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The passwords are the same one')</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>478</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="C162" t="s">
+        <v>480</v>
+      </c>
+      <c r="D162" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.pass.no.coinciden',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Las contraseñas son no coinciden')</v>
+      </c>
+      <c r="E162" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.pass.no.coinciden',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The passwords don´t match')</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>482</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="C163" t="s">
+        <v>484</v>
+      </c>
+      <c r="D163" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.permisos.esenciales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Se perderian permisos esenciales')</v>
+      </c>
+      <c r="E163" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.permisos.esenciales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Essential roles would be lost')</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>485</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="C164" t="s">
+        <v>487</v>
+      </c>
+      <c r="D164" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.path',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Seleccione una ruta')</v>
+      </c>
+      <c r="E164" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.path',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Select a path')</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>488</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="C165" t="s">
+        <v>490</v>
+      </c>
+      <c r="D165" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.mail.invalido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Mail inválido')</v>
+      </c>
+      <c r="E165" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.mail.invalido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Invalid mail')</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="2"/>
+      <c r="D166" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E166" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D167" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E167" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D168" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E168" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D169" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E169" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D170" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E170" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D171" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E171" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D172" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E172" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D173" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E173" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D174" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E174" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D175" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E175" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D176" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E176" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="177" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D177" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E177" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="178" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D178" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E178" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="179" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D179" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E179" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="180" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D180" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E180" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="181" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D181" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E181" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="182" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D182" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E182" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="183" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D183" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E183" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="184" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D184" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E184" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="185" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D185" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E185" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="186" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D186" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E186" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="187" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D187" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E187" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="188" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D188" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E188" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="189" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D189" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E189" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="190" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D190" t="str">
+        <f t="shared" ref="D190:D253" si="6">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+values ('",
+$A190,
+"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
+$D$1,
+"'),'",
+$B190,
+"')"))</f>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E190" t="str">
+        <f t="shared" ref="E190:E253" si="7">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+values ('",
+$A190,
+"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
+$E$1,
+"'),'",
+$C190,
+"')"))</f>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="191" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D191" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E191" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="192" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D192" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E192" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="193" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D193" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E193" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="194" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D194" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E194" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="195" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D195" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E195" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="196" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D196" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E196" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="197" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D197" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E197" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="198" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D198" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E198" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="199" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D199" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E199" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="200" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D200" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E200" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="201" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D201" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E201" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="202" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D202" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E202" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="203" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D203" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E203" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="204" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D204" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E204" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="205" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D205" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E205" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="206" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D206" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E206" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="207" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D207" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E207" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="208" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D208" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E208" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="209" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D209" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E209" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="210" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D210" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E210" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="211" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D211" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E211" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="212" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D212" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E212" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="213" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D213" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E213" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="214" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D214" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E214" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="215" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D215" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E215" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="216" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D216" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E216" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="217" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D217" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E217" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="218" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D218" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E218" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="219" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D219" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E219" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="220" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D220" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E220" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="221" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D221" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E221" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="222" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D222" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E222" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="223" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D223" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E223" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="224" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D224" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E224" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="225" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D225" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E225" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="226" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D226" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E226" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="227" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D227" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E227" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="228" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D228" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E228" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="229" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D229" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E229" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="230" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D230" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E230" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="231" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D231" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E231" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="232" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D232" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E232" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="233" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D233" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E233" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="234" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D234" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E234" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="235" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D235" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E235" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="236" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D236" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E236" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="237" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D237" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E237" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="238" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D238" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E238" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="239" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D239" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E239" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="240" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D240" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E240" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="241" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D241" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E241" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="242" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D242" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E242" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="243" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D243" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E243" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="244" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D244" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E244" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="245" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D245" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E245" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="246" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D246" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E246" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="247" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D247" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E247" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="248" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D248" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E248" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="249" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D249" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E249" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="250" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D250" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E250" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="251" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D251" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E251" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="252" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D252" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E252" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="253" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D253" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E253" t="str">
+        <f t="shared" si="7"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="254" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D254" t="str">
+        <f t="shared" ref="D254:D270" si="8">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+values ('",
+$A254,
+"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
+$D$1,
+"'),'",
+$B254,
+"')"))</f>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E254" t="str">
+        <f t="shared" ref="E254:E270" si="9">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+values ('",
+$A254,
+"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
+$E$1,
+"'),'",
+$C254,
+"')"))</f>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="255" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D255" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E255" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="256" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D256" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E256" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="257" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D257" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E257" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="258" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D258" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E258" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="259" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D259" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E259" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="260" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D260" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E260" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="261" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D261" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E261" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="262" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D262" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E262" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="263" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D263" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E263" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="264" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D264" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E264" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="265" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D265" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E265" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="266" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D266" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E266" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="267" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D267" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E267" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="268" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D268" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E268" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="269" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D269" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E269" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+      </c>
+    </row>
+    <row r="270" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D270" t="str">
+        <f t="shared" si="8"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+      </c>
+      <c r="E270" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
       </c>
     </row>
   </sheetData>
@@ -3953,21 +6212,21 @@
         <v>44</v>
       </c>
       <c r="D1" t="s">
+        <v>342</v>
+      </c>
+      <c r="E1" t="s">
         <v>343</v>
-      </c>
-      <c r="E1" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C2" t="s">
         <v>374</v>
-      </c>
-      <c r="C2" t="s">
-        <v>375</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D7" si="0">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
@@ -3994,13 +6253,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B3" t="s">
         <v>357</v>
       </c>
-      <c r="B3" t="s">
-        <v>358</v>
-      </c>
       <c r="C3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
@@ -4013,13 +6272,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>361</v>
+      </c>
+      <c r="B4" t="s">
         <v>362</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>363</v>
-      </c>
-      <c r="C4" t="s">
-        <v>364</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
@@ -4032,13 +6291,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>364</v>
+      </c>
+      <c r="B5" t="s">
         <v>365</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>366</v>
-      </c>
-      <c r="C5" t="s">
-        <v>367</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
@@ -4051,13 +6310,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>367</v>
+      </c>
+      <c r="B6" t="s">
         <v>368</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>369</v>
-      </c>
-      <c r="C6" t="s">
-        <v>370</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -4070,13 +6329,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>370</v>
+      </c>
+      <c r="B7" t="s">
         <v>371</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>372</v>
-      </c>
-      <c r="C7" t="s">
-        <v>373</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
-- logueo de bitacora -- modificacion en abm usuario no actualizaba la lista despues de hacer alta o mod -- fixed no se calculaba el digito vertical en alta de usu, y no se asignaban los permisos. -- fixed filtrado y muestra de nulos en bitacora
</commit_message>
<xml_diff>
--- a/Varios/traducciones.xlsx
+++ b/Varios/traducciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Documents\Trabajo-De-Campo\trabajo-de-diploma\Varios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3709192C-1B55-4266-937E-7A172A77A702}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A3C974-5F57-44B1-84C4-3B2CE4ED5584}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{461B7C5F-BDDA-470F-86DF-9E00192D23ED}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="491">
   <si>
     <t>Alumno</t>
   </si>
@@ -1471,9 +1471,6 @@
     <t>com.td.pass.no.coinciden</t>
   </si>
   <si>
-    <t>Las contraseñas son no coinciden</t>
-  </si>
-  <si>
     <t>The passwords don´t match</t>
   </si>
   <si>
@@ -1505,22 +1502,17 @@
   </si>
   <si>
     <t>Invalid mail</t>
+  </si>
+  <si>
+    <t>Las contraseñas  no coinciden</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1548,10 +1540,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1867,10 +1858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB4AC18-9E40-4F52-A240-1F2EFB37F2BC}">
-  <dimension ref="A1:E270"/>
+  <dimension ref="A1:E167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E131" workbookViewId="0">
-      <selection activeCell="D148" sqref="D148:E165"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A148" sqref="A148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4355,7 +4346,7 @@
         <v>381</v>
       </c>
       <c r="D127" t="str">
-        <f t="shared" ref="D127:D189" si="4">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+        <f t="shared" ref="D127:D167" si="4">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
 values ('",
 $A127,
 "',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
@@ -4366,7 +4357,7 @@
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.motivo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Motivo')</v>
       </c>
       <c r="E127" t="str">
-        <f t="shared" ref="E127:E189" si="5">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+        <f t="shared" ref="E127:E167" si="5">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
 values ('",
 $A127,
 "',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
@@ -4492,7 +4483,7 @@
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" s="3" t="s">
+      <c r="A134" s="2" t="s">
         <v>398</v>
       </c>
       <c r="B134" t="s">
@@ -4511,7 +4502,7 @@
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" s="3" t="s">
+      <c r="A135" s="2" t="s">
         <v>401</v>
       </c>
       <c r="B135" t="s">
@@ -4530,10 +4521,10 @@
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" s="3" t="s">
+      <c r="A136" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B136" s="3" t="s">
+      <c r="B136" s="2" t="s">
         <v>404</v>
       </c>
       <c r="C136" t="s">
@@ -4549,10 +4540,10 @@
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" s="3" t="s">
+      <c r="A137" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="B137" s="3" t="s">
+      <c r="B137" s="2" t="s">
         <v>408</v>
       </c>
       <c r="C137" t="s">
@@ -4568,10 +4559,10 @@
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" s="3" t="s">
+      <c r="A138" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B138" s="3" t="s">
+      <c r="B138" s="2" t="s">
         <v>413</v>
       </c>
       <c r="C138" t="s">
@@ -4587,10 +4578,10 @@
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" s="3" t="s">
+      <c r="A139" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="B139" s="3" t="s">
+      <c r="B139" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C139" t="s">
@@ -4606,10 +4597,10 @@
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" s="3" t="s">
+      <c r="A140" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="B140" s="3" t="s">
+      <c r="B140" s="2" t="s">
         <v>414</v>
       </c>
       <c r="C140" t="s">
@@ -4625,10 +4616,10 @@
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" s="3" t="s">
+      <c r="A141" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="B141" s="3" t="s">
+      <c r="B141" s="2" t="s">
         <v>419</v>
       </c>
       <c r="C141" t="s">
@@ -4704,7 +4695,7 @@
       <c r="A145" t="s">
         <v>429</v>
       </c>
-      <c r="B145" s="3" t="s">
+      <c r="B145" s="2" t="s">
         <v>430</v>
       </c>
       <c r="C145" t="s">
@@ -4723,7 +4714,7 @@
       <c r="A146" t="s">
         <v>432</v>
       </c>
-      <c r="B146" s="3" t="s">
+      <c r="B146" s="2" t="s">
         <v>433</v>
       </c>
       <c r="C146" t="s">
@@ -4742,7 +4733,7 @@
       <c r="A147" t="s">
         <v>434</v>
       </c>
-      <c r="B147" s="3" t="s">
+      <c r="B147" s="2" t="s">
         <v>435</v>
       </c>
       <c r="C147" t="s">
@@ -4761,8 +4752,8 @@
       <c r="A148" t="s">
         <v>437</v>
       </c>
-      <c r="B148" s="3" t="s">
-        <v>481</v>
+      <c r="B148" s="2" t="s">
+        <v>480</v>
       </c>
       <c r="C148" t="s">
         <v>459</v>
@@ -4780,7 +4771,7 @@
       <c r="A149" t="s">
         <v>438</v>
       </c>
-      <c r="B149" s="3" t="s">
+      <c r="B149" s="2" t="s">
         <v>439</v>
       </c>
       <c r="C149" t="s">
@@ -4799,7 +4790,7 @@
       <c r="A150" t="s">
         <v>441</v>
       </c>
-      <c r="B150" s="3" t="s">
+      <c r="B150" s="2" t="s">
         <v>442</v>
       </c>
       <c r="C150" t="s">
@@ -4818,7 +4809,7 @@
       <c r="A151" t="s">
         <v>444</v>
       </c>
-      <c r="B151" s="3" t="s">
+      <c r="B151" s="2" t="s">
         <v>445</v>
       </c>
       <c r="C151" t="s">
@@ -4837,7 +4828,7 @@
       <c r="A152" t="s">
         <v>447</v>
       </c>
-      <c r="B152" s="3" t="s">
+      <c r="B152" s="2" t="s">
         <v>448</v>
       </c>
       <c r="C152" t="s">
@@ -4856,7 +4847,7 @@
       <c r="A153" t="s">
         <v>450</v>
       </c>
-      <c r="B153" s="3" t="s">
+      <c r="B153" s="2" t="s">
         <v>452</v>
       </c>
       <c r="C153" t="s">
@@ -4875,7 +4866,7 @@
       <c r="A154" t="s">
         <v>453</v>
       </c>
-      <c r="B154" s="3" t="s">
+      <c r="B154" s="2" t="s">
         <v>454</v>
       </c>
       <c r="C154" t="s">
@@ -4894,7 +4885,7 @@
       <c r="A155" t="s">
         <v>456</v>
       </c>
-      <c r="B155" s="3" t="s">
+      <c r="B155" s="2" t="s">
         <v>457</v>
       </c>
       <c r="C155" t="s">
@@ -4913,7 +4904,7 @@
       <c r="A156" t="s">
         <v>460</v>
       </c>
-      <c r="B156" s="3" t="s">
+      <c r="B156" s="2" t="s">
         <v>461</v>
       </c>
       <c r="C156" t="s">
@@ -4932,7 +4923,7 @@
       <c r="A157" t="s">
         <v>463</v>
       </c>
-      <c r="B157" s="3" t="s">
+      <c r="B157" s="2" t="s">
         <v>464</v>
       </c>
       <c r="C157" t="s">
@@ -4951,7 +4942,7 @@
       <c r="A158" t="s">
         <v>466</v>
       </c>
-      <c r="B158" s="3" t="s">
+      <c r="B158" s="2" t="s">
         <v>467</v>
       </c>
       <c r="C158" t="s">
@@ -4970,7 +4961,7 @@
       <c r="A159" t="s">
         <v>469</v>
       </c>
-      <c r="B159" s="3" t="s">
+      <c r="B159" s="2" t="s">
         <v>470</v>
       </c>
       <c r="C159" t="s">
@@ -4989,7 +4980,7 @@
       <c r="A160" t="s">
         <v>472</v>
       </c>
-      <c r="B160" s="3" t="s">
+      <c r="B160" s="2" t="s">
         <v>473</v>
       </c>
       <c r="C160" t="s">
@@ -5008,7 +4999,7 @@
       <c r="A161" t="s">
         <v>475</v>
       </c>
-      <c r="B161" s="3" t="s">
+      <c r="B161" s="2" t="s">
         <v>476</v>
       </c>
       <c r="C161" t="s">
@@ -5027,15 +5018,15 @@
       <c r="A162" t="s">
         <v>478</v>
       </c>
-      <c r="B162" s="3" t="s">
+      <c r="B162" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="C162" t="s">
         <v>479</v>
-      </c>
-      <c r="C162" t="s">
-        <v>480</v>
       </c>
       <c r="D162" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.pass.no.coinciden',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Las contraseñas son no coinciden')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.pass.no.coinciden',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Las contraseñas  no coinciden')</v>
       </c>
       <c r="E162" t="str">
         <f t="shared" si="5"/>
@@ -5044,13 +5035,13 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
+        <v>481</v>
+      </c>
+      <c r="B163" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="B163" s="3" t="s">
+      <c r="C163" t="s">
         <v>483</v>
-      </c>
-      <c r="C163" t="s">
-        <v>484</v>
       </c>
       <c r="D163" t="str">
         <f t="shared" si="4"/>
@@ -5063,13 +5054,13 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
+        <v>484</v>
+      </c>
+      <c r="B164" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="B164" s="3" t="s">
+      <c r="C164" t="s">
         <v>486</v>
-      </c>
-      <c r="C164" t="s">
-        <v>487</v>
       </c>
       <c r="D164" t="str">
         <f t="shared" si="4"/>
@@ -5082,13 +5073,13 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
+        <v>487</v>
+      </c>
+      <c r="B165" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="B165" s="3" t="s">
+      <c r="C165" t="s">
         <v>489</v>
-      </c>
-      <c r="C165" t="s">
-        <v>490</v>
       </c>
       <c r="D165" t="str">
         <f t="shared" si="4"/>
@@ -5100,1082 +5091,41 @@
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" s="2"/>
+      <c r="A166" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B166" t="s">
+        <v>362</v>
+      </c>
+      <c r="C166" t="s">
+        <v>363</v>
+      </c>
       <c r="D166" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.header',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Su cuenta fue creada con éxito')</v>
       </c>
       <c r="E166" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.header',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Your account was created successfully')</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>364</v>
+      </c>
+      <c r="B167" t="s">
+        <v>365</v>
+      </c>
+      <c r="C167" t="s">
+        <v>366</v>
+      </c>
       <c r="D167" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.body',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Esta es su contraseña:')</v>
       </c>
       <c r="E167" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D168" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E168" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D169" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E169" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D170" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E170" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D171" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E171" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D172" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E172" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D173" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E173" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D174" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E174" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D175" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E175" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D176" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E176" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="177" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D177" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E177" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="178" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D178" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E178" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="179" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D179" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E179" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="180" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D180" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E180" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="181" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D181" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E181" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="182" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D182" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E182" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="183" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D183" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E183" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="184" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D184" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E184" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="185" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D185" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E185" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="186" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D186" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E186" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="187" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D187" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E187" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="188" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D188" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E188" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="189" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D189" t="str">
-        <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E189" t="str">
-        <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="190" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D190" t="str">
-        <f t="shared" ref="D190:D253" si="6">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
-values ('",
-$A190,
-"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
-$D$1,
-"'),'",
-$B190,
-"')"))</f>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E190" t="str">
-        <f t="shared" ref="E190:E253" si="7">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
-values ('",
-$A190,
-"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
-$E$1,
-"'),'",
-$C190,
-"')"))</f>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="191" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D191" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E191" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="192" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D192" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E192" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="193" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D193" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E193" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="194" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D194" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E194" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="195" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D195" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E195" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="196" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D196" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E196" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="197" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D197" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E197" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="198" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D198" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E198" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="199" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D199" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E199" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="200" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D200" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E200" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="201" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D201" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E201" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="202" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D202" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E202" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="203" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D203" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E203" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="204" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D204" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E204" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="205" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D205" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E205" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="206" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D206" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E206" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="207" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D207" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E207" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="208" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D208" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E208" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="209" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D209" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E209" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="210" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D210" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E210" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="211" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D211" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E211" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="212" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D212" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E212" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="213" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D213" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E213" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="214" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D214" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E214" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="215" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D215" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E215" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="216" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D216" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E216" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="217" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D217" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E217" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="218" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D218" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E218" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="219" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D219" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E219" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="220" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D220" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E220" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="221" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D221" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E221" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="222" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D222" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E222" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="223" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D223" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E223" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="224" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D224" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E224" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="225" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D225" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E225" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="226" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D226" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E226" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="227" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D227" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E227" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="228" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D228" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E228" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="229" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D229" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E229" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="230" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D230" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E230" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="231" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D231" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E231" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="232" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D232" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E232" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="233" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D233" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E233" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="234" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D234" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E234" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="235" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D235" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E235" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="236" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D236" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E236" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="237" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D237" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E237" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="238" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D238" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E238" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="239" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D239" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E239" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="240" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D240" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E240" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="241" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D241" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E241" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="242" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D242" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E242" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="243" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D243" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E243" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="244" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D244" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E244" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="245" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D245" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E245" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="246" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D246" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E246" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="247" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D247" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E247" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="248" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D248" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E248" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="249" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D249" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E249" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="250" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D250" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E250" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="251" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D251" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E251" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="252" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D252" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E252" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="253" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D253" t="str">
-        <f t="shared" si="6"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E253" t="str">
-        <f t="shared" si="7"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="254" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D254" t="str">
-        <f t="shared" ref="D254:D270" si="8">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
-values ('",
-$A254,
-"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
-$D$1,
-"'),'",
-$B254,
-"')"))</f>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E254" t="str">
-        <f t="shared" ref="E254:E270" si="9">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
-values ('",
-$A254,
-"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
-$E$1,
-"'),'",
-$C254,
-"')"))</f>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="255" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D255" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E255" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="256" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D256" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E256" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="257" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D257" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E257" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="258" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D258" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E258" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="259" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D259" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E259" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="260" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D260" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E260" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="261" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D261" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E261" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="262" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D262" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E262" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="263" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D263" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E263" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="264" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D264" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E264" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="265" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D265" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E265" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="266" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D266" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E266" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="267" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D267" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E267" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="268" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D268" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E268" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="269" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D269" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E269" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
-      </c>
-    </row>
-    <row r="270" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D270" t="str">
-        <f t="shared" si="8"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'')</v>
-      </c>
-      <c r="E270" t="str">
-        <f t="shared" si="9"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.body',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'This is your password:')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-- agregue la verificacion de permisos esenciales en mod familia -- chequee donde falta tocar los ds y donde faltan message boxes
</commit_message>
<xml_diff>
--- a/Varios/traducciones.xlsx
+++ b/Varios/traducciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Documents\Trabajo-De-Campo\trabajo-de-diploma\Varios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A3C974-5F57-44B1-84C4-3B2CE4ED5584}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F2E3F2-1A92-4E16-A36B-C173048A33C1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{461B7C5F-BDDA-470F-86DF-9E00192D23ED}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="506">
   <si>
     <t>Alumno</t>
   </si>
@@ -1505,6 +1505,51 @@
   </si>
   <si>
     <t>Las contraseñas  no coinciden</t>
+  </si>
+  <si>
+    <t>com.td.horario.no.disponible</t>
+  </si>
+  <si>
+    <t>Horario no disponible</t>
+  </si>
+  <si>
+    <t>Schedule not available</t>
+  </si>
+  <si>
+    <t>com.td.curso.codigo.existe</t>
+  </si>
+  <si>
+    <t>Código existente</t>
+  </si>
+  <si>
+    <t>The code already exists</t>
+  </si>
+  <si>
+    <t>com.td.curso.tiene.alumnos</t>
+  </si>
+  <si>
+    <t>Tiene alumnos</t>
+  </si>
+  <si>
+    <t>It has students</t>
+  </si>
+  <si>
+    <t>com.td.repetidos</t>
+  </si>
+  <si>
+    <t>El mail o el D.N.I. ya existe</t>
+  </si>
+  <si>
+    <t>The mail or the ID already exist</t>
+  </si>
+  <si>
+    <t>com.td.familia.existe</t>
+  </si>
+  <si>
+    <t>El nombre de la familia existe</t>
+  </si>
+  <si>
+    <t>The family name already exists</t>
   </si>
 </sst>
 </file>
@@ -1858,10 +1903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB4AC18-9E40-4F52-A240-1F2EFB37F2BC}">
-  <dimension ref="A1:E167"/>
+  <dimension ref="A1:E172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A148" sqref="A148"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4346,7 +4391,7 @@
         <v>381</v>
       </c>
       <c r="D127" t="str">
-        <f t="shared" ref="D127:D167" si="4">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+        <f t="shared" ref="D127:D172" si="4">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
 values ('",
 $A127,
 "',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
@@ -4357,7 +4402,7 @@
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.motivo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Motivo')</v>
       </c>
       <c r="E127" t="str">
-        <f t="shared" ref="E127:E167" si="5">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+        <f t="shared" ref="E127:E172" si="5">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
 values ('",
 $A127,
 "',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
@@ -5126,6 +5171,101 @@
       <c r="E167" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.body',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'This is your password:')</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>491</v>
+      </c>
+      <c r="B168" t="s">
+        <v>492</v>
+      </c>
+      <c r="C168" t="s">
+        <v>493</v>
+      </c>
+      <c r="D168" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.horario.no.disponible',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Horario no disponible')</v>
+      </c>
+      <c r="E168" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.horario.no.disponible',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Schedule not available')</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>494</v>
+      </c>
+      <c r="B169" t="s">
+        <v>495</v>
+      </c>
+      <c r="C169" t="s">
+        <v>496</v>
+      </c>
+      <c r="D169" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.curso.codigo.existe',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Código existente')</v>
+      </c>
+      <c r="E169" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.curso.codigo.existe',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The code already exists')</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>497</v>
+      </c>
+      <c r="B170" t="s">
+        <v>498</v>
+      </c>
+      <c r="C170" t="s">
+        <v>499</v>
+      </c>
+      <c r="D170" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.curso.tiene.alumnos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Tiene alumnos')</v>
+      </c>
+      <c r="E170" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.curso.tiene.alumnos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'It has students')</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>500</v>
+      </c>
+      <c r="B171" t="s">
+        <v>501</v>
+      </c>
+      <c r="C171" t="s">
+        <v>502</v>
+      </c>
+      <c r="D171" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.repetidos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'El mail o el D.N.I. ya existe')</v>
+      </c>
+      <c r="E171" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.repetidos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The mail or the ID already exist')</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>503</v>
+      </c>
+      <c r="B172" t="s">
+        <v>504</v>
+      </c>
+      <c r="C172" t="s">
+        <v>505</v>
+      </c>
+      <c r="D172" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.familia.existe',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'El nombre de la familia existe')</v>
+      </c>
+      <c r="E172" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.familia.existe',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The family name already exists')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
----mensajes metidos cu backup falta confirmacion cu restore falta confirmacion cu borrar horario agregar pedido de confirmacion cu borrar curso pedir confirmacion cu registar amonestacion pedir confirmacion cu registar/modificar inasistencia inasistencia pedir confirmacion cu borrar tutor pedir confirmacion. borrar tutor mejore mensaje de excepcion cu log out pedir confirmacion
</commit_message>
<xml_diff>
--- a/Varios/traducciones.xlsx
+++ b/Varios/traducciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Documents\Trabajo-De-Campo\trabajo-de-diploma\Varios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F2E3F2-1A92-4E16-A36B-C173048A33C1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F1CF46-5F3B-484F-8CC2-063EC7663E92}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{461B7C5F-BDDA-470F-86DF-9E00192D23ED}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="512">
   <si>
     <t>Alumno</t>
   </si>
@@ -1550,6 +1550,24 @@
   </si>
   <si>
     <t>The family name already exists</t>
+  </si>
+  <si>
+    <t>com.td.seguro</t>
+  </si>
+  <si>
+    <t>¿Está seguro?</t>
+  </si>
+  <si>
+    <t>Are you sure?</t>
+  </si>
+  <si>
+    <t>com.td.tutor.asignado</t>
+  </si>
+  <si>
+    <t>El tutor esta asignado</t>
+  </si>
+  <si>
+    <t>The tutor is assigned</t>
   </si>
 </sst>
 </file>
@@ -1903,10 +1921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB4AC18-9E40-4F52-A240-1F2EFB37F2BC}">
-  <dimension ref="A1:E172"/>
+  <dimension ref="A1:E173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="D166" workbookViewId="0">
+      <selection activeCell="E172" sqref="D172:E172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4315,14 +4333,14 @@
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
-        <v>126</v>
+      <c r="A125" t="s">
+        <v>376</v>
       </c>
       <c r="B125" t="s">
-        <v>9</v>
+        <v>377</v>
       </c>
       <c r="C125" t="s">
-        <v>243</v>
+        <v>378</v>
       </c>
       <c r="D125" t="str">
         <f>CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
@@ -4333,7 +4351,7 @@
 "'),'",
 $B125,
 "')"))</f>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.asignado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Asignado')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.valor',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Valor')</v>
       </c>
       <c r="E125" t="str">
         <f>CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
@@ -4344,21 +4362,21 @@
 "'),'",
 $C125,
 "')"))</f>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.asignado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Assigned')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.valor',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Value')</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>376</v>
+      <c r="A126" s="1" t="s">
+        <v>379</v>
       </c>
       <c r="B126" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="C126" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="D126" t="str">
-        <f>CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+        <f t="shared" ref="D126:D173" si="4">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
 values ('",
 $A126,
 "',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
@@ -4366,10 +4384,10 @@
 "'),'",
 $B126,
 "')"))</f>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.valor',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Valor')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.motivo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Motivo')</v>
       </c>
       <c r="E126" t="str">
-        <f>CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+        <f t="shared" ref="E126:E173" si="5">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
 values ('",
 $A126,
 "',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
@@ -4377,895 +4395,900 @@
 "'),'",
 $C126,
 "')"))</f>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.valor',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Value')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.motivo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Reason')</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
-        <v>379</v>
+      <c r="A127" t="s">
+        <v>382</v>
       </c>
       <c r="B127" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="C127" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="D127" t="str">
-        <f t="shared" ref="D127:D172" si="4">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
-values ('",
-$A127,
-"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
-$D$1,
-"'),'",
-$B127,
-"')"))</f>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.motivo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Motivo')</v>
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.crear',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Crear')</v>
       </c>
       <c r="E127" t="str">
-        <f t="shared" ref="E127:E172" si="5">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
-values ('",
-$A127,
-"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
-$E$1,
-"'),'",
-$C127,
-"')"))</f>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.motivo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Reason')</v>
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.crear',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Create')</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="B128" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="C128" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D128" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.crear',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Crear')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.niveles',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Niveles')</v>
       </c>
       <c r="E128" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.crear',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Create')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.niveles',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Levels')</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="B129" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C129" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="D129" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.niveles',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Niveles')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tipo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Tipo')</v>
       </c>
       <c r="E129" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.niveles',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Levels')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tipo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Type')</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="B130" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C130" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="D130" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tipo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Tipo')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.egresar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Egresar')</v>
       </c>
       <c r="E130" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tipo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Type')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.egresar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Graduate')</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>391</v>
+        <v>207</v>
       </c>
       <c r="B131" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C131" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="D131" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.egresar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Egresar')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.promocionar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Promocionar')</v>
       </c>
       <c r="E131" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.egresar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Graduate')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.promocionar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Promote')</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>207</v>
+      <c r="A132" s="1" t="s">
+        <v>396</v>
       </c>
       <c r="B132" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="C132" t="s">
-        <v>395</v>
+        <v>360</v>
       </c>
       <c r="D132" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.promocionar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Promocionar')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.bloqueado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Bloqueado')</v>
       </c>
       <c r="E132" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.promocionar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Promote')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.bloqueado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Blocked')</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
-        <v>396</v>
+      <c r="A133" s="2" t="s">
+        <v>398</v>
       </c>
       <c r="B133" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C133" t="s">
-        <v>360</v>
+        <v>400</v>
       </c>
       <c r="D133" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.bloqueado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Bloqueado')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.si',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Sí')</v>
       </c>
       <c r="E133" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.bloqueado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Blocked')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.si',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Yes')</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="B134" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="C134" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="D134" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.si',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Sí')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.no',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'No')</v>
       </c>
       <c r="E134" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.si',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Yes')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.no',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'No')</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="B135" t="s">
-        <v>402</v>
+        <v>406</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>404</v>
       </c>
       <c r="C135" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="D135" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.no',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'No')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.generate.respaldo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Generar Respaldo')</v>
       </c>
       <c r="E135" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.no',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'No')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.generate.respaldo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Generate Backup')</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="C136" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="D136" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.generate.respaldo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Generar Respaldo')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.contiene',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Contiene')</v>
       </c>
       <c r="E136" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.generate.respaldo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Generate Backup')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.contiene',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Contains')</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="C137" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="D137" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.contiene',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Contiene')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.alta',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Alta')</v>
       </c>
       <c r="E137" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.contiene',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Contains')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.alta',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'High')</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>413</v>
+        <v>31</v>
       </c>
       <c r="C138" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D138" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.alta',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Alta')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.media',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Media')</v>
       </c>
       <c r="E138" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.alta',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'High')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.media',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Medium')</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>31</v>
+        <v>414</v>
       </c>
       <c r="C139" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D139" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.media',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Media')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.baja',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Baja')</v>
       </c>
       <c r="E139" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.media',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Medium')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.baja',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Low')</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="C140" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="D140" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.baja',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Baja')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.menu',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Gestión Educativa')</v>
       </c>
       <c r="E140" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.baja',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Low')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.menu',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Education Management')</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>419</v>
+      <c r="A141" t="s">
+        <v>422</v>
+      </c>
+      <c r="B141" t="s">
+        <v>421</v>
       </c>
       <c r="C141" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D141" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.menu',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Gestión Educativa')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Tutor')</v>
       </c>
       <c r="E141" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.menu',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Education Management')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Tutor')</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B142" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="C142" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="D142" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Tutor')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.faltas.totales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Faltas Totales')</v>
       </c>
       <c r="E142" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Tutor')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.faltas.totales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Total Abscences')</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="B143" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="C143" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D143" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.faltas.totales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Faltas Totales')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.disclaimer',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Los cursos marcados en rojo se estan excedidos')</v>
       </c>
       <c r="E143" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.faltas.totales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Total Abscences')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.disclaimer',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The courses marked with red are exceeded')</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>426</v>
-      </c>
-      <c r="B144" t="s">
-        <v>428</v>
+        <v>429</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>430</v>
       </c>
       <c r="C144" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="D144" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.disclaimer',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Los cursos marcados en rojo se estan excedidos')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.maximo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Máximo')</v>
       </c>
       <c r="E144" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.disclaimer',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The courses marked with red are exceeded')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.maximo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Maximum')</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="C145" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="D145" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.maximo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Máximo')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.actual',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Actual')</v>
       </c>
       <c r="E145" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.maximo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Maximum')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.actual',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Actual')</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C146" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="D146" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.actual',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Actual')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.plan.estudios',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Plan de estudios')</v>
       </c>
       <c r="E146" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.actual',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Actual')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.plan.estudios',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Curriculum')</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>435</v>
+        <v>480</v>
       </c>
       <c r="C147" t="s">
-        <v>436</v>
+        <v>459</v>
       </c>
       <c r="D147" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.plan.estudios',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Plan de estudios')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.complete.campos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Complete todos los campos requeridos')</v>
       </c>
       <c r="E147" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.plan.estudios',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Curriculum')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.complete.campos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Complete all the required fields')</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>480</v>
+        <v>439</v>
       </c>
       <c r="C148" t="s">
-        <v>459</v>
+        <v>440</v>
       </c>
       <c r="D148" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.complete.campos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Complete todos los campos requeridos')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.completado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Completado')</v>
       </c>
       <c r="E148" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.complete.campos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Complete all the required fields')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.completado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Completed')</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="C149" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="D149" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.completado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Completado')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.existe.materia',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Ya existe la materia')</v>
       </c>
       <c r="E149" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.completado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Completed')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.existe.materia',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The class already exists')</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="C150" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="D150" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.existe.materia',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Ya existe la materia')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.descartar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Descartar cambios')</v>
       </c>
       <c r="E150" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.existe.materia',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The class already exists')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.descartar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'DiscardChanges')</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="C151" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="D151" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.descartar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Descartar cambios')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seleccione.horario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Seleccione un horario')</v>
       </c>
       <c r="E151" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.descartar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'DiscardChanges')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seleccione.horario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Select a schedule')</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="C152" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D152" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seleccione.horario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Seleccione un horario')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.falta.horario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'No hay un horario ahí')</v>
       </c>
       <c r="E152" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seleccione.horario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Select a schedule')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.falta.horario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'There is no schedule there')</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C153" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="D153" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.falta.horario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'No hay un horario ahí')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.materia.asignada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'La materia esta asignada')</v>
       </c>
       <c r="E153" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.falta.horario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'There is no schedule there')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.materia.asignada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The class is assigned')</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="C154" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="D154" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.materia.asignada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'La materia esta asignada')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seleccione.busqueda',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Seleccione datos de busqueda')</v>
       </c>
       <c r="E154" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.materia.asignada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The class is assigned')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seleccione.busqueda',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Select something to search by')</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="C155" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="D155" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seleccione.busqueda',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Seleccione datos de busqueda')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.orientacion.incorrecta',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'La orientacion no corresponde al curso')</v>
       </c>
       <c r="E155" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seleccione.busqueda',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Select something to search by')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.orientacion.incorrecta',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The course does not have that orientation')</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="C156" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="D156" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.orientacion.incorrecta',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'La orientacion no corresponde al curso')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor.requerido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Se requiere al menos un tutor')</v>
       </c>
       <c r="E156" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.orientacion.incorrecta',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The course does not have that orientation')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor.requerido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'At least one tutor required')</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="C157" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="D157" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor.requerido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Se requiere al menos un tutor')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.dni.repetido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'D.N.I. ya existente')</v>
       </c>
       <c r="E157" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor.requerido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'At least one tutor required')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.dni.repetido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'ID already exists')</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="C158" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="D158" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.dni.repetido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'D.N.I. ya existente')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.fecha.ocupada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Fecha ocupada')</v>
       </c>
       <c r="E158" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.dni.repetido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'ID already exists')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.fecha.ocupada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Date already entered')</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="C159" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="D159" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.fecha.ocupada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Fecha ocupada')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.char.count',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Como mínimo 8 caracteres')</v>
       </c>
       <c r="E159" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.fecha.ocupada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Date already entered')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.char.count',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'At least 8 characters')</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="C160" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="D160" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.char.count',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Como mínimo 8 caracteres')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.pass.iguales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Las contraseñas son iguales')</v>
       </c>
       <c r="E160" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.char.count',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'At least 8 characters')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.pass.iguales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The passwords are the same one')</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>476</v>
+        <v>490</v>
       </c>
       <c r="C161" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="D161" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.pass.iguales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Las contraseñas son iguales')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.pass.no.coinciden',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Las contraseñas  no coinciden')</v>
       </c>
       <c r="E161" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.pass.iguales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The passwords are the same one')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.pass.no.coinciden',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The passwords don´t match')</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="C162" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="D162" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.pass.no.coinciden',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Las contraseñas  no coinciden')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.permisos.esenciales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Se perderian permisos esenciales')</v>
       </c>
       <c r="E162" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.pass.no.coinciden',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The passwords don´t match')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.permisos.esenciales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Essential roles would be lost')</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="C163" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="D163" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.permisos.esenciales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Se perderian permisos esenciales')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.path',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Seleccione una ruta')</v>
       </c>
       <c r="E163" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.permisos.esenciales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Essential roles would be lost')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.path',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Select a path')</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="C164" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="D164" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.path',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Seleccione una ruta')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.mail.invalido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Mail inválido')</v>
       </c>
       <c r="E164" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.path',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Select a path')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.mail.invalido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Invalid mail')</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>487</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>488</v>
+      <c r="A165" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B165" t="s">
+        <v>362</v>
       </c>
       <c r="C165" t="s">
-        <v>489</v>
+        <v>363</v>
       </c>
       <c r="D165" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.mail.invalido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Mail inválido')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.header',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Su cuenta fue creada con éxito')</v>
       </c>
       <c r="E165" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.mail.invalido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Invalid mail')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.header',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Your account was created successfully')</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" s="2" t="s">
-        <v>361</v>
+      <c r="A166" t="s">
+        <v>364</v>
       </c>
       <c r="B166" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="C166" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="D166" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.header',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Su cuenta fue creada con éxito')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.body',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Esta es su contraseña:')</v>
       </c>
       <c r="E166" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.header',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Your account was created successfully')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.body',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'This is your password:')</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>364</v>
+        <v>491</v>
       </c>
       <c r="B167" t="s">
-        <v>365</v>
+        <v>492</v>
       </c>
       <c r="C167" t="s">
-        <v>366</v>
+        <v>493</v>
       </c>
       <c r="D167" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.body',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Esta es su contraseña:')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.horario.no.disponible',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Horario no disponible')</v>
       </c>
       <c r="E167" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.body',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'This is your password:')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.horario.no.disponible',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Schedule not available')</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="B168" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="C168" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="D168" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.horario.no.disponible',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Horario no disponible')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.curso.codigo.existe',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Código existente')</v>
       </c>
       <c r="E168" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.horario.no.disponible',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Schedule not available')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.curso.codigo.existe',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The code already exists')</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="B169" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="C169" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="D169" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.curso.codigo.existe',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Código existente')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.curso.tiene.alumnos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Tiene alumnos')</v>
       </c>
       <c r="E169" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.curso.codigo.existe',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The code already exists')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.curso.tiene.alumnos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'It has students')</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="B170" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="C170" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="D170" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.curso.tiene.alumnos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Tiene alumnos')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.repetidos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'El mail o el D.N.I. ya existe')</v>
       </c>
       <c r="E170" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.curso.tiene.alumnos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'It has students')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.repetidos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The mail or the ID already exist')</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="B171" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="C171" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="D171" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.repetidos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'El mail o el D.N.I. ya existe')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.familia.existe',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'El nombre de la familia existe')</v>
       </c>
       <c r="E171" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.repetidos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The mail or the ID already exist')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.familia.existe',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The family name already exists')</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="B172" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="C172" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="D172" t="str">
         <f t="shared" si="4"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.familia.existe',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'El nombre de la familia existe')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seguro',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'¿Está seguro?')</v>
       </c>
       <c r="E172" t="str">
         <f t="shared" si="5"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.familia.existe',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The family name already exists')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seguro',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Are you sure?')</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>509</v>
+      </c>
+      <c r="B173" t="s">
+        <v>510</v>
+      </c>
+      <c r="C173" t="s">
+        <v>511</v>
+      </c>
+      <c r="D173" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor.asignado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'El tutor esta asignado')</v>
+      </c>
+      <c r="E173" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor.asignado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The tutor is assigned')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-- no permitir el bloqueo o borrado de uno mismo -- cambio para bloquear al usuario inclusive si es admin -- cambio para tomar el backspace en falla de conexion -- nuevos mensajes
</commit_message>
<xml_diff>
--- a/Varios/traducciones.xlsx
+++ b/Varios/traducciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Documents\Trabajo-De-Campo\trabajo-de-diploma\Varios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Documents\TrabajoDeCampo\trabajo-de-diploma\Varios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F1CF46-5F3B-484F-8CC2-063EC7663E92}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC4FB60-79BF-4EEE-9333-C91E7C3CA420}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{461B7C5F-BDDA-470F-86DF-9E00192D23ED}"/>
   </bookViews>
@@ -24,7 +24,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="515">
   <si>
     <t>Alumno</t>
   </si>
@@ -1568,6 +1567,15 @@
   </si>
   <si>
     <t>The tutor is assigned</t>
+  </si>
+  <si>
+    <t>com.td.mismo.usuario</t>
+  </si>
+  <si>
+    <t>No puede borrarse o bloquearse a si mismo</t>
+  </si>
+  <si>
+    <t>You can´t delete or block yourself</t>
   </si>
 </sst>
 </file>
@@ -1921,10 +1929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB4AC18-9E40-4F52-A240-1F2EFB37F2BC}">
-  <dimension ref="A1:E173"/>
+  <dimension ref="A1:E174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D166" workbookViewId="0">
-      <selection activeCell="E172" sqref="D172:E172"/>
+    <sheetView tabSelected="1" topLeftCell="E166" workbookViewId="0">
+      <selection activeCell="D174" sqref="D174:E174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4376,7 +4384,7 @@
         <v>381</v>
       </c>
       <c r="D126" t="str">
-        <f t="shared" ref="D126:D173" si="4">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+        <f t="shared" ref="D126:D174" si="4">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
 values ('",
 $A126,
 "',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
@@ -4387,7 +4395,7 @@
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.motivo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Motivo')</v>
       </c>
       <c r="E126" t="str">
-        <f t="shared" ref="E126:E173" si="5">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+        <f t="shared" ref="E126:E174" si="5">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
 values ('",
 $A126,
 "',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
@@ -5289,6 +5297,25 @@
       <c r="E173" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor.asignado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The tutor is assigned')</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>512</v>
+      </c>
+      <c r="B174" t="s">
+        <v>513</v>
+      </c>
+      <c r="C174" t="s">
+        <v>514</v>
+      </c>
+      <c r="D174" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.mismo.usuario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'No puede borrarse o bloquearse a si mismo')</v>
+      </c>
+      <c r="E174" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.mismo.usuario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'You can´t delete or block yourself')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-- correciones que faltaban con respecto a mensajes y balanceo con la carpeta
</commit_message>
<xml_diff>
--- a/Varios/traducciones.xlsx
+++ b/Varios/traducciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Documents\TrabajoDeCampo\trabajo-de-diploma\Varios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Documents\Trabajo-De-Campo\trabajo-de-diploma\Varios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC4FB60-79BF-4EEE-9333-C91E7C3CA420}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0344DCED-8AB4-4239-83E0-66ED63BB2B06}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{461B7C5F-BDDA-470F-86DF-9E00192D23ED}"/>
   </bookViews>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="518">
   <si>
     <t>Alumno</t>
   </si>
@@ -1576,6 +1577,15 @@
   </si>
   <si>
     <t>You can´t delete or block yourself</t>
+  </si>
+  <si>
+    <t>com.td.excedido</t>
+  </si>
+  <si>
+    <t>La capacidad del curso fue excedida</t>
+  </si>
+  <si>
+    <t>The course capacity is over the limit</t>
   </si>
 </sst>
 </file>
@@ -1929,10 +1939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB4AC18-9E40-4F52-A240-1F2EFB37F2BC}">
-  <dimension ref="A1:E174"/>
+  <dimension ref="A1:E175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E166" workbookViewId="0">
-      <selection activeCell="D174" sqref="D174:E174"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="A175" sqref="A175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4384,7 +4394,7 @@
         <v>381</v>
       </c>
       <c r="D126" t="str">
-        <f t="shared" ref="D126:D174" si="4">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+        <f t="shared" ref="D126:D175" si="4">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
 values ('",
 $A126,
 "',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
@@ -4395,7 +4405,7 @@
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.motivo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Motivo')</v>
       </c>
       <c r="E126" t="str">
-        <f t="shared" ref="E126:E174" si="5">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+        <f t="shared" ref="E126:E175" si="5">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
 values ('",
 $A126,
 "',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
@@ -5316,6 +5326,25 @@
       <c r="E174" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.mismo.usuario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'You can´t delete or block yourself')</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>515</v>
+      </c>
+      <c r="B175" t="s">
+        <v>516</v>
+      </c>
+      <c r="C175" t="s">
+        <v>517</v>
+      </c>
+      <c r="D175" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.excedido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'La capacidad del curso fue excedida')</v>
+      </c>
+      <c r="E175" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.excedido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The course capacity is over the limit')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
--correcciones de la primera entrega formal
</commit_message>
<xml_diff>
--- a/Varios/traducciones.xlsx
+++ b/Varios/traducciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Documents\Trabajo-De-Campo\trabajo-de-diploma\Varios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0344DCED-8AB4-4239-83E0-66ED63BB2B06}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4A32BC-24C0-47E1-807D-20C1D5776819}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{461B7C5F-BDDA-470F-86DF-9E00192D23ED}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Controles" sheetId="1" r:id="rId1"/>
     <sheet name="Mensajes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="524">
   <si>
     <t>Alumno</t>
   </si>
@@ -1586,6 +1586,24 @@
   </si>
   <si>
     <t>The course capacity is over the limit</t>
+  </si>
+  <si>
+    <t>com.td.desbloquear</t>
+  </si>
+  <si>
+    <t>Desbloquear</t>
+  </si>
+  <si>
+    <t>Unlock</t>
+  </si>
+  <si>
+    <t>Rango de fechas inválido</t>
+  </si>
+  <si>
+    <t>Invalid Date Range</t>
+  </si>
+  <si>
+    <t>com.td.rango.fecha.invalido</t>
   </si>
 </sst>
 </file>
@@ -1939,10 +1957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB4AC18-9E40-4F52-A240-1F2EFB37F2BC}">
-  <dimension ref="A1:E175"/>
+  <dimension ref="A1:E177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="A175" sqref="A175"/>
+    <sheetView tabSelected="1" topLeftCell="E164" workbookViewId="0">
+      <selection activeCell="D177" sqref="D177:E177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3212,7 +3230,7 @@
         <v>290</v>
       </c>
       <c r="D66" t="str">
-        <f t="shared" ref="D66:D123" si="2">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+        <f t="shared" ref="D66:D124" si="2">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
 values ('",
 $A66,
 "',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
@@ -3223,7 +3241,7 @@
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.conectar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Conectar')</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" ref="E66:E123" si="3">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+        <f t="shared" ref="E66:E124" si="3">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
 values ('",
 $A66,
 "',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
@@ -3274,1091 +3292,1077 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>223</v>
+        <v>518</v>
       </c>
       <c r="B69" t="s">
-        <v>63</v>
+        <v>519</v>
       </c>
       <c r="C69" t="s">
-        <v>293</v>
+        <v>520</v>
       </c>
       <c r="D69" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.regenerar.password',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Regenerar Password')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.desbloquear',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Desbloquear')</v>
       </c>
       <c r="E69" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.regenerar.password',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Regenerate password')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.desbloquear',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Unlock')</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B70" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C70" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.patentes.asignadas',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Patentes Asignadas')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.regenerar.password',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Regenerar Password')</v>
       </c>
       <c r="E70" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.patentes.asignadas',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Assigned Patents')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.regenerar.password',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Regenerate password')</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B71" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C71" t="s">
-        <v>403</v>
+        <v>294</v>
       </c>
       <c r="D71" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.respaldo.base.de.datos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Respaldo Base de Datos')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.patentes.asignadas',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Patentes Asignadas')</v>
       </c>
       <c r="E71" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.respaldo.base.de.datos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Database backup')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.patentes.asignadas',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Assigned Patents')</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>168</v>
+        <v>225</v>
       </c>
       <c r="B72" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C72" t="s">
-        <v>66</v>
+        <v>403</v>
       </c>
       <c r="D72" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.login',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Login')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.respaldo.base.de.datos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Respaldo Base de Datos')</v>
       </c>
       <c r="E72" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.login',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Login')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.respaldo.base.de.datos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Database backup')</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>226</v>
+        <v>168</v>
       </c>
       <c r="B73" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C73" t="s">
-        <v>295</v>
+        <v>66</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seleccione.destino',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Seleccione destino')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.login',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Login')</v>
       </c>
       <c r="E73" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seleccione.destino',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Select destination')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.login',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Login')</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B74" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C74" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.cantidad.de.partes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Cantidad de partes')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seleccione.destino',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Seleccione destino')</v>
       </c>
       <c r="E74" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.cantidad.de.partes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Number of parts')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seleccione.destino',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Select destination')</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>169</v>
+        <v>227</v>
       </c>
       <c r="B75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C75" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.examinar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Examinar')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.cantidad.de.partes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Cantidad de partes')</v>
       </c>
       <c r="E75" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.examinar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Examine')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.cantidad.de.partes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Number of parts')</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B76" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C76" t="s">
-        <v>80</v>
+        <v>297</v>
       </c>
       <c r="D76" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.respaldar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Respaldar')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.examinar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Examinar')</v>
       </c>
       <c r="E76" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.respaldar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Backup')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.examinar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Examine')</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>228</v>
+        <v>170</v>
       </c>
       <c r="B77" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C77" t="s">
-        <v>298</v>
+        <v>80</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.restaurar.backup',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Restaurar Backup')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.respaldar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Respaldar')</v>
       </c>
       <c r="E77" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.restaurar.backup',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Restore backup')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.respaldar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Backup')</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>171</v>
+        <v>228</v>
       </c>
       <c r="B78" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C78" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.origen',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Origen')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.restaurar.backup',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Restaurar Backup')</v>
       </c>
       <c r="E78" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.origen',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Origin')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.restaurar.backup',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Restore backup')</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B79" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C79" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.restaurar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Restaurar')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.origen',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Origen')</v>
       </c>
       <c r="E79" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.restaurar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Restore')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.origen',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Origin')</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B80" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C80" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D80" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.docentes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Docentes ')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.restaurar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Restaurar')</v>
       </c>
       <c r="E80" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.docentes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Teachers')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.restaurar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Restore')</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B81" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C81" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D81" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.notas',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Notas')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.docentes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Docentes ')</v>
       </c>
       <c r="E81" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.notas',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Grades')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.docentes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Teachers')</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B82" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C82" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.reportes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Reportes')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.notas',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Notas')</v>
       </c>
       <c r="E82" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.reportes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Reports')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.notas',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Grades')</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B83" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C83" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D83" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.administración',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Administración')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.reportes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Reportes')</v>
       </c>
       <c r="E83" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.administración',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Administration')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.reportes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Reports')</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B84" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C84" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D84" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seguridad',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Seguridad')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.administración',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Administración')</v>
       </c>
       <c r="E84" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seguridad',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Security')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.administración',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Administration')</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B85" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C85" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D85" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.permisos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Permisos')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seguridad',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Seguridad')</v>
       </c>
       <c r="E85" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.permisos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Permissions')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seguridad',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Security')</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B86" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C86" t="s">
-        <v>80</v>
+        <v>306</v>
       </c>
       <c r="D86" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.backup',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Backup')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.permisos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Permisos')</v>
       </c>
       <c r="E86" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.backup',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Backup')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.permisos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Permissions')</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>229</v>
+        <v>179</v>
       </c>
       <c r="B87" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C87" t="s">
-        <v>307</v>
+        <v>80</v>
       </c>
       <c r="D87" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.recalcular.dígitos.verificadores',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Recalcular Dígitos Verificadores')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.backup',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Backup')</v>
       </c>
       <c r="E87" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.recalcular.dígitos.verificadores',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Recalculate verification digits')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.backup',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Backup')</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>180</v>
+        <v>229</v>
       </c>
       <c r="B88" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C88" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D88" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.opciones',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Opciones')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.recalcular.dígitos.verificadores',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Recalcular Dígitos Verificadores')</v>
       </c>
       <c r="E88" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.opciones',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Options')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.recalcular.dígitos.verificadores',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Recalculate verification digits')</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>230</v>
+        <v>180</v>
       </c>
       <c r="B89" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C89" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D89" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.cambiar.idioma',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Cambiar Idioma')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.opciones',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Opciones')</v>
       </c>
       <c r="E89" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.cambiar.idioma',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Change Language')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.opciones',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Options')</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B90" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C90" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D90" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.cerrar.sesion',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Cerrar Sesion')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.cambiar.idioma',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Cambiar Idioma')</v>
       </c>
       <c r="E90" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.cerrar.sesion',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Close session')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.cambiar.idioma',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Change Language')</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>181</v>
+        <v>231</v>
       </c>
       <c r="B91" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C91" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D91" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.salir',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Salir')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.cerrar.sesion',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Cerrar Sesion')</v>
       </c>
       <c r="E91" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.salir',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Exit')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.cerrar.sesion',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Close session')</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B92" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C92" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D92" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.capacidad',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Capacidad')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.salir',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Salir')</v>
       </c>
       <c r="E92" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.capacidad',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Capacity')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.salir',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Exit')</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B93" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C93" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D93" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.letra',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Letra')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.capacidad',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Capacidad')</v>
       </c>
       <c r="E93" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.letra',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Letter')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.capacidad',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Capacity')</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B94" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C94" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D94" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.mañana',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Mañana')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.letra',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Letra')</v>
       </c>
       <c r="E94" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.mañana',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Morning')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.letra',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Letter')</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B95" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C95" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D95" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tarde',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Tarde')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.mañana',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Mañana')</v>
       </c>
       <c r="E95" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tarde',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Afternoon')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.mañana',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Morning')</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B96" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C96" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D96" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.turno',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Turno')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tarde',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Tarde')</v>
       </c>
       <c r="E96" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.turno',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Shift')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tarde',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Afternoon')</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B97" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C97" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D97" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.nivel',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Nivel')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.turno',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Turno')</v>
       </c>
       <c r="E97" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.nivel',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Level')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.turno',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Shift')</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B98" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C98" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D98" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.docente',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Docente')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.nivel',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Nivel')</v>
       </c>
       <c r="E98" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.docente',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Teacher')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.nivel',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Level')</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B99" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C99" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D99" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.materia',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Materia')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.docente',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Docente')</v>
       </c>
       <c r="E99" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.materia',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Class')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.docente',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Teacher')</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B100" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C100" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D100" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.día',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Día')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.materia',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Materia')</v>
       </c>
       <c r="E100" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.día',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Day')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.materia',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Class')</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B101" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C101" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D101" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.módulo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Módulo')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.día',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Día')</v>
       </c>
       <c r="E101" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.módulo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Module')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.día',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Day')</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B102" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C102" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D102" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.horario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Horario')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.módulo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Módulo')</v>
       </c>
       <c r="E102" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.horario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Schedule')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.módulo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Module')</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B103" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C103" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D103" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.extracurricular',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Extracurricular ')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.horario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Horario')</v>
       </c>
       <c r="E103" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.extracurricular',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Extracurricular')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.horario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Schedule')</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B104" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C104" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D104" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.troncal',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Troncal')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.extracurricular',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Extracurricular ')</v>
       </c>
       <c r="E104" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.troncal',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Core')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.extracurricular',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Extracurricular')</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="B105" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C105" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D105" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.asignación.de.materias',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Asignación de Materias')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.troncal',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Troncal')</v>
       </c>
       <c r="E105" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.asignación.de.materias',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Class Assignment')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.troncal',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Core')</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
       <c r="B106" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C106" t="s">
-        <v>243</v>
+        <v>325</v>
       </c>
       <c r="D106" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.asignadas',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Asignadas')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.asignación.de.materias',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Asignación de Materias')</v>
       </c>
       <c r="E106" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.asignadas',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Assigned')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.asignación.de.materias',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Class Assignment')</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B107" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C107" t="s">
-        <v>326</v>
+        <v>243</v>
       </c>
       <c r="D107" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.asignar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Asignar')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.asignadas',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Asignadas')</v>
       </c>
       <c r="E107" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.asignar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Assign')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.asignadas',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Assigned')</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B108" t="s">
-        <v>328</v>
+        <v>101</v>
       </c>
       <c r="C108" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D108" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.desasignar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Desasignar')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.asignar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Asignar')</v>
       </c>
       <c r="E108" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.desasignar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Deassign')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.asignar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Assign')</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>232</v>
+        <v>197</v>
       </c>
       <c r="B109" t="s">
-        <v>102</v>
+        <v>328</v>
       </c>
       <c r="C109" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D109" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.sin.asignar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Sin Asignar')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.desasignar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Desasignar')</v>
       </c>
       <c r="E109" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.sin.asignar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Unassigned')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.desasignar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Deassign')</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="B110" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C110" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D110" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.cursos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Cursos')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.sin.asignar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Sin Asignar')</v>
       </c>
       <c r="E110" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.cursos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Courses')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.sin.asignar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Unassigned')</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B111" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C111" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D111" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.código',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Código')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.cursos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Cursos')</v>
       </c>
       <c r="E111" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.código',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Code')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.cursos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Courses')</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B112" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C112" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D112" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.lunes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Lunes')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.código',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Código')</v>
       </c>
       <c r="E112" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.lunes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Monday')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.código',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Code')</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B113" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C113" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D113" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.martes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Martes')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.lunes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Lunes')</v>
       </c>
       <c r="E113" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.martes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Tuesday')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.lunes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Monday')</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B114" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C114" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D114" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.miercoles',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Miercoles')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.martes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Martes')</v>
       </c>
       <c r="E114" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.miercoles',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Wednesday')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.martes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Tuesday')</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B115" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C115" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D115" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.jueves',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Jueves ')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.miercoles',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Miercoles')</v>
       </c>
       <c r="E115" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.jueves',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Thurdsday')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.miercoles',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Wednesday')</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B116" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C116" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D116" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.viernes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Viernes')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.jueves',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Jueves ')</v>
       </c>
       <c r="E116" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.viernes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Friday')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.jueves',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Thurdsday')</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B117" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C117" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D117" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.horarios',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Horarios')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.viernes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Viernes')</v>
       </c>
       <c r="E117" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.horarios',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Schedules')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.viernes',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Friday')</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B118" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C118" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D118" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.materias',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Materias')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.horarios',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Horarios')</v>
       </c>
       <c r="E118" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.materias',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Classes')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.horarios',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Schedules')</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B119" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C119" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D119" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.promoción.de.alumnos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Promoción de Alumnos')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.materias',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Materias')</v>
       </c>
       <c r="E119" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.promoción.de.alumnos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Student Promotions')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.materias',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Classes')</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>233</v>
+        <v>211</v>
       </c>
       <c r="B120" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C120" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D120" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.promocionar.al.curso',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Promocionar al curso')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.promoción.de.alumnos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Promoción de Alumnos')</v>
       </c>
       <c r="E120" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.promocionar.al.curso',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Promote to Class')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.promoción.de.alumnos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Student Promotions')</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>207</v>
+        <v>233</v>
       </c>
       <c r="B121" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C121" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D121" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.promocionar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'PROMOCIONAR')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.promocionar.al.curso',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Promocionar al curso')</v>
       </c>
       <c r="E121" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.promocionar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'PROMOTE')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.promocionar.al.curso',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Promote to Class')</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>347</v>
+        <v>207</v>
       </c>
       <c r="B122" t="s">
-        <v>348</v>
+        <v>114</v>
       </c>
       <c r="C122" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="D122" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.ayuda',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Ayuda')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.promocionar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'PROMOCIONAR')</v>
       </c>
       <c r="E122" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.ayuda',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Help')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.promocionar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'PROMOTE')</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B123" t="s">
-        <v>94</v>
+        <v>348</v>
       </c>
       <c r="C123" t="s">
-        <v>320</v>
+        <v>349</v>
       </c>
       <c r="D123" t="str">
         <f t="shared" si="2"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.dia',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Día')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.ayuda',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Ayuda')</v>
       </c>
       <c r="E123" t="str">
         <f t="shared" si="3"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.dia',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Day')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.ayuda',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Help')</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B124" t="s">
-        <v>353</v>
+        <v>94</v>
       </c>
       <c r="C124" t="s">
-        <v>354</v>
+        <v>320</v>
       </c>
       <c r="D124" t="str">
-        <f>CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
-values ('",
-$A124,
-"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
-$D$1,
-"'),'",
-$B124,
-"')"))</f>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.repetir',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Repetir')</v>
+        <f t="shared" si="2"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.dia',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Día')</v>
       </c>
       <c r="E124" t="str">
-        <f>CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
-values ('",
-$A124,
-"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
-$E$1,
-"'),'",
-$C124,
-"')"))</f>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.repetir',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Fail Course')</v>
+        <f t="shared" si="3"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.dia',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Day')</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>376</v>
+        <v>352</v>
       </c>
       <c r="B125" t="s">
-        <v>377</v>
+        <v>353</v>
       </c>
       <c r="C125" t="s">
-        <v>378</v>
+        <v>354</v>
       </c>
       <c r="D125" t="str">
         <f>CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
@@ -4369,7 +4373,7 @@
 "'),'",
 $B125,
 "')"))</f>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.valor',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Valor')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.repetir',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Repetir')</v>
       </c>
       <c r="E125" t="str">
         <f>CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
@@ -4380,21 +4384,21 @@
 "'),'",
 $C125,
 "')"))</f>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.valor',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Value')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.repetir',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Fail Course')</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
-        <v>379</v>
+      <c r="A126" t="s">
+        <v>376</v>
       </c>
       <c r="B126" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C126" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D126" t="str">
-        <f t="shared" ref="D126:D175" si="4">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+        <f>CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
 values ('",
 $A126,
 "',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
@@ -4402,10 +4406,10 @@
 "'),'",
 $B126,
 "')"))</f>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.motivo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Motivo')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.valor',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Valor')</v>
       </c>
       <c r="E126" t="str">
-        <f t="shared" ref="E126:E175" si="5">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+        <f>CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
 values ('",
 $A126,
 "',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
@@ -4413,938 +4417,990 @@
 "'),'",
 $C126,
 "')"))</f>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.valor',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Value')</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B127" t="s">
+        <v>380</v>
+      </c>
+      <c r="C127" t="s">
+        <v>381</v>
+      </c>
+      <c r="D127" t="str">
+        <f t="shared" ref="D127:D177" si="4">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+values ('",
+$A127,
+"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
+$D$1,
+"'),'",
+$B127,
+"')"))</f>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.motivo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Motivo')</v>
+      </c>
+      <c r="E127" t="str">
+        <f t="shared" ref="E127:E177" si="5">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+values ('",
+$A127,
+"',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
+$E$1,
+"'),'",
+$C127,
+"')"))</f>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.motivo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Reason')</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>382</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B128" t="s">
         <v>383</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C128" t="s">
         <v>384</v>
       </c>
-      <c r="D127" t="str">
+      <c r="D128" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.crear',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Crear')</v>
       </c>
-      <c r="E127" t="str">
+      <c r="E128" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.crear',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Create')</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>385</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B129" t="s">
         <v>387</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C129" t="s">
         <v>386</v>
       </c>
-      <c r="D128" t="str">
+      <c r="D129" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.niveles',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Niveles')</v>
       </c>
-      <c r="E128" t="str">
+      <c r="E129" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.niveles',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Levels')</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>388</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B130" t="s">
         <v>389</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C130" t="s">
         <v>390</v>
       </c>
-      <c r="D129" t="str">
+      <c r="D130" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tipo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Tipo')</v>
       </c>
-      <c r="E129" t="str">
+      <c r="E130" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tipo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Type')</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>391</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B131" t="s">
         <v>392</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C131" t="s">
         <v>393</v>
       </c>
-      <c r="D130" t="str">
+      <c r="D131" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.egresar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Egresar')</v>
       </c>
-      <c r="E130" t="str">
+      <c r="E131" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.egresar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Graduate')</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>207</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B132" t="s">
         <v>394</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C132" t="s">
         <v>395</v>
       </c>
-      <c r="D131" t="str">
+      <c r="D132" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.promocionar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Promocionar')</v>
       </c>
-      <c r="E131" t="str">
+      <c r="E132" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.promocionar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Promote')</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B133" t="s">
         <v>397</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C133" t="s">
         <v>360</v>
       </c>
-      <c r="D132" t="str">
+      <c r="D133" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.bloqueado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Bloqueado')</v>
       </c>
-      <c r="E132" t="str">
+      <c r="E133" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.bloqueado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Blocked')</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B134" t="s">
         <v>399</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C134" t="s">
         <v>400</v>
       </c>
-      <c r="D133" t="str">
+      <c r="D134" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.si',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Sí')</v>
       </c>
-      <c r="E133" t="str">
+      <c r="E134" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.si',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Yes')</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" s="2" t="s">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B135" t="s">
         <v>402</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C135" t="s">
         <v>402</v>
       </c>
-      <c r="D134" t="str">
+      <c r="D135" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.no',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'No')</v>
       </c>
-      <c r="E134" t="str">
+      <c r="E135" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.no',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'No')</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="B136" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C136" t="s">
         <v>405</v>
       </c>
-      <c r="D135" t="str">
+      <c r="D136" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.generate.respaldo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Generar Respaldo')</v>
       </c>
-      <c r="E135" t="str">
+      <c r="E136" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.generate.respaldo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Generate Backup')</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" s="2" t="s">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="B137" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C137" t="s">
         <v>409</v>
       </c>
-      <c r="D136" t="str">
+      <c r="D137" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.contiene',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Contiene')</v>
       </c>
-      <c r="E136" t="str">
+      <c r="E137" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.contiene',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Contains')</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="B138" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C138" t="s">
         <v>415</v>
       </c>
-      <c r="D137" t="str">
+      <c r="D138" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.alta',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Alta')</v>
       </c>
-      <c r="E137" t="str">
+      <c r="E138" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.alta',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'High')</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="B138" s="2" t="s">
+      <c r="B139" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C139" t="s">
         <v>416</v>
       </c>
-      <c r="D138" t="str">
+      <c r="D139" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.media',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Media')</v>
       </c>
-      <c r="E138" t="str">
+      <c r="E139" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.media',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Medium')</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="B140" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C140" t="s">
         <v>417</v>
       </c>
-      <c r="D139" t="str">
+      <c r="D140" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.baja',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Baja')</v>
       </c>
-      <c r="E139" t="str">
+      <c r="E140" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.criticidad.baja',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Low')</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" s="2" t="s">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="B141" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C141" t="s">
         <v>420</v>
       </c>
-      <c r="D140" t="str">
+      <c r="D141" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.menu',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Gestión Educativa')</v>
       </c>
-      <c r="E140" t="str">
+      <c r="E141" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.menu',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Education Management')</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>422</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B142" t="s">
         <v>421</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C142" t="s">
         <v>421</v>
       </c>
-      <c r="D141" t="str">
+      <c r="D142" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Tutor')</v>
       </c>
-      <c r="E141" t="str">
+      <c r="E142" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Tutor')</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>423</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B143" t="s">
         <v>424</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C143" t="s">
         <v>425</v>
       </c>
-      <c r="D142" t="str">
+      <c r="D143" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.faltas.totales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Faltas Totales')</v>
       </c>
-      <c r="E142" t="str">
+      <c r="E143" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.faltas.totales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Total Abscences')</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>426</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B144" t="s">
         <v>428</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C144" t="s">
         <v>427</v>
       </c>
-      <c r="D143" t="str">
+      <c r="D144" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.disclaimer',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Los cursos marcados en rojo se estan excedidos')</v>
       </c>
-      <c r="E143" t="str">
+      <c r="E144" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.disclaimer',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The courses marked with red are exceeded')</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>429</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="B145" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C145" t="s">
         <v>431</v>
       </c>
-      <c r="D144" t="str">
+      <c r="D145" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.maximo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Máximo')</v>
       </c>
-      <c r="E144" t="str">
+      <c r="E145" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.maximo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Maximum')</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>432</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="B146" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C146" t="s">
         <v>433</v>
       </c>
-      <c r="D145" t="str">
+      <c r="D146" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.actual',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Actual')</v>
       </c>
-      <c r="E145" t="str">
+      <c r="E146" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.actual',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Actual')</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>434</v>
       </c>
-      <c r="B146" s="2" t="s">
+      <c r="B147" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C147" t="s">
         <v>436</v>
       </c>
-      <c r="D146" t="str">
+      <c r="D147" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.plan.estudios',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Plan de estudios')</v>
       </c>
-      <c r="E146" t="str">
+      <c r="E147" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.plan.estudios',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Curriculum')</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>437</v>
       </c>
-      <c r="B147" s="2" t="s">
+      <c r="B148" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C148" t="s">
         <v>459</v>
       </c>
-      <c r="D147" t="str">
+      <c r="D148" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.complete.campos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Complete todos los campos requeridos')</v>
       </c>
-      <c r="E147" t="str">
+      <c r="E148" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.complete.campos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Complete all the required fields')</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>438</v>
       </c>
-      <c r="B148" s="2" t="s">
+      <c r="B149" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C149" t="s">
         <v>440</v>
       </c>
-      <c r="D148" t="str">
+      <c r="D149" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.completado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Completado')</v>
       </c>
-      <c r="E148" t="str">
+      <c r="E149" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.completado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Completed')</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>441</v>
       </c>
-      <c r="B149" s="2" t="s">
+      <c r="B150" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C150" t="s">
         <v>443</v>
       </c>
-      <c r="D149" t="str">
+      <c r="D150" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.existe.materia',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Ya existe la materia')</v>
       </c>
-      <c r="E149" t="str">
+      <c r="E150" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.existe.materia',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The class already exists')</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>444</v>
       </c>
-      <c r="B150" s="2" t="s">
+      <c r="B151" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C151" t="s">
         <v>446</v>
       </c>
-      <c r="D150" t="str">
+      <c r="D151" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.descartar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Descartar cambios')</v>
       </c>
-      <c r="E150" t="str">
+      <c r="E151" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.descartar',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'DiscardChanges')</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>447</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="B152" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C152" t="s">
         <v>449</v>
       </c>
-      <c r="D151" t="str">
+      <c r="D152" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seleccione.horario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Seleccione un horario')</v>
       </c>
-      <c r="E151" t="str">
+      <c r="E152" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seleccione.horario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Select a schedule')</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>450</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="B153" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="C152" t="s">
+      <c r="C153" t="s">
         <v>451</v>
       </c>
-      <c r="D152" t="str">
+      <c r="D153" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.falta.horario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'No hay un horario ahí')</v>
       </c>
-      <c r="E152" t="str">
+      <c r="E153" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.falta.horario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'There is no schedule there')</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>453</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="B154" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C154" t="s">
         <v>455</v>
       </c>
-      <c r="D153" t="str">
+      <c r="D154" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.materia.asignada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'La materia esta asignada')</v>
       </c>
-      <c r="E153" t="str">
+      <c r="E154" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.materia.asignada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The class is assigned')</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>456</v>
       </c>
-      <c r="B154" s="2" t="s">
+      <c r="B155" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C155" t="s">
         <v>458</v>
       </c>
-      <c r="D154" t="str">
+      <c r="D155" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seleccione.busqueda',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Seleccione datos de busqueda')</v>
       </c>
-      <c r="E154" t="str">
+      <c r="E155" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seleccione.busqueda',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Select something to search by')</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>460</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="B156" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C156" t="s">
         <v>462</v>
       </c>
-      <c r="D155" t="str">
+      <c r="D156" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.orientacion.incorrecta',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'La orientacion no corresponde al curso')</v>
       </c>
-      <c r="E155" t="str">
+      <c r="E156" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.orientacion.incorrecta',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The course does not have that orientation')</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>463</v>
       </c>
-      <c r="B156" s="2" t="s">
+      <c r="B157" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C157" t="s">
         <v>465</v>
       </c>
-      <c r="D156" t="str">
+      <c r="D157" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor.requerido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Se requiere al menos un tutor')</v>
       </c>
-      <c r="E156" t="str">
+      <c r="E157" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor.requerido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'At least one tutor required')</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>466</v>
       </c>
-      <c r="B157" s="2" t="s">
+      <c r="B158" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C158" t="s">
         <v>468</v>
       </c>
-      <c r="D157" t="str">
+      <c r="D158" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.dni.repetido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'D.N.I. ya existente')</v>
       </c>
-      <c r="E157" t="str">
+      <c r="E158" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.dni.repetido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'ID already exists')</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>469</v>
       </c>
-      <c r="B158" s="2" t="s">
+      <c r="B159" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C159" t="s">
         <v>471</v>
       </c>
-      <c r="D158" t="str">
+      <c r="D159" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.fecha.ocupada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Fecha ocupada')</v>
       </c>
-      <c r="E158" t="str">
+      <c r="E159" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.fecha.ocupada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Date already entered')</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>472</v>
       </c>
-      <c r="B159" s="2" t="s">
+      <c r="B160" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C160" t="s">
         <v>474</v>
       </c>
-      <c r="D159" t="str">
+      <c r="D160" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.char.count',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Como mínimo 8 caracteres')</v>
       </c>
-      <c r="E159" t="str">
+      <c r="E160" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.char.count',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'At least 8 characters')</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>475</v>
       </c>
-      <c r="B160" s="2" t="s">
+      <c r="B161" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C161" t="s">
         <v>477</v>
       </c>
-      <c r="D160" t="str">
+      <c r="D161" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.pass.iguales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Las contraseñas son iguales')</v>
       </c>
-      <c r="E160" t="str">
+      <c r="E161" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.pass.iguales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The passwords are the same one')</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>478</v>
       </c>
-      <c r="B161" s="2" t="s">
+      <c r="B162" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C162" t="s">
         <v>479</v>
       </c>
-      <c r="D161" t="str">
+      <c r="D162" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.pass.no.coinciden',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Las contraseñas  no coinciden')</v>
       </c>
-      <c r="E161" t="str">
+      <c r="E162" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.pass.no.coinciden',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The passwords don´t match')</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>481</v>
       </c>
-      <c r="B162" s="2" t="s">
+      <c r="B163" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C163" t="s">
         <v>483</v>
       </c>
-      <c r="D162" t="str">
+      <c r="D163" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.permisos.esenciales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Se perderian permisos esenciales')</v>
       </c>
-      <c r="E162" t="str">
+      <c r="E163" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.permisos.esenciales',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Essential roles would be lost')</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>484</v>
       </c>
-      <c r="B163" s="2" t="s">
+      <c r="B164" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C164" t="s">
         <v>486</v>
       </c>
-      <c r="D163" t="str">
+      <c r="D164" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.path',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Seleccione una ruta')</v>
       </c>
-      <c r="E163" t="str">
+      <c r="E164" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.path',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Select a path')</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>487</v>
       </c>
-      <c r="B164" s="2" t="s">
+      <c r="B165" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C165" t="s">
         <v>489</v>
       </c>
-      <c r="D164" t="str">
+      <c r="D165" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.mail.invalido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Mail inválido')</v>
       </c>
-      <c r="E164" t="str">
+      <c r="E165" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.mail.invalido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Invalid mail')</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" s="2" t="s">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B166" t="s">
         <v>362</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C166" t="s">
         <v>363</v>
       </c>
-      <c r="D165" t="str">
+      <c r="D166" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.header',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Su cuenta fue creada con éxito')</v>
       </c>
-      <c r="E165" t="str">
+      <c r="E166" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.header',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Your account was created successfully')</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>364</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B167" t="s">
         <v>365</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C167" t="s">
         <v>366</v>
       </c>
-      <c r="D166" t="str">
+      <c r="D167" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.body',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Esta es su contraseña:')</v>
       </c>
-      <c r="E166" t="str">
+      <c r="E167" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.body',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'This is your password:')</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>491</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B168" t="s">
         <v>492</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C168" t="s">
         <v>493</v>
       </c>
-      <c r="D167" t="str">
+      <c r="D168" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.horario.no.disponible',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Horario no disponible')</v>
       </c>
-      <c r="E167" t="str">
+      <c r="E168" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.horario.no.disponible',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Schedule not available')</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>494</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B169" t="s">
         <v>495</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C169" t="s">
         <v>496</v>
       </c>
-      <c r="D168" t="str">
+      <c r="D169" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.curso.codigo.existe',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Código existente')</v>
       </c>
-      <c r="E168" t="str">
+      <c r="E169" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.curso.codigo.existe',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The code already exists')</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>497</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B170" t="s">
         <v>498</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C170" t="s">
         <v>499</v>
       </c>
-      <c r="D169" t="str">
+      <c r="D170" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.curso.tiene.alumnos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Tiene alumnos')</v>
       </c>
-      <c r="E169" t="str">
+      <c r="E170" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.curso.tiene.alumnos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'It has students')</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
         <v>500</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B171" t="s">
         <v>501</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C171" t="s">
         <v>502</v>
       </c>
-      <c r="D170" t="str">
+      <c r="D171" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.repetidos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'El mail o el D.N.I. ya existe')</v>
       </c>
-      <c r="E170" t="str">
+      <c r="E171" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.repetidos',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The mail or the ID already exist')</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
         <v>503</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B172" t="s">
         <v>504</v>
       </c>
-      <c r="C171" t="s">
+      <c r="C172" t="s">
         <v>505</v>
       </c>
-      <c r="D171" t="str">
+      <c r="D172" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.familia.existe',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'El nombre de la familia existe')</v>
       </c>
-      <c r="E171" t="str">
+      <c r="E172" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.familia.existe',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The family name already exists')</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>506</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B173" t="s">
         <v>507</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C173" t="s">
         <v>508</v>
       </c>
-      <c r="D172" t="str">
+      <c r="D173" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seguro',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'¿Está seguro?')</v>
       </c>
-      <c r="E172" t="str">
+      <c r="E173" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.seguro',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Are you sure?')</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
         <v>509</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B174" t="s">
         <v>510</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C174" t="s">
         <v>511</v>
       </c>
-      <c r="D173" t="str">
+      <c r="D174" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor.asignado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'El tutor esta asignado')</v>
       </c>
-      <c r="E173" t="str">
+      <c r="E174" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.tutor.asignado',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The tutor is assigned')</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>512</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B175" t="s">
         <v>513</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C175" t="s">
         <v>514</v>
       </c>
-      <c r="D174" t="str">
+      <c r="D175" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.mismo.usuario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'No puede borrarse o bloquearse a si mismo')</v>
       </c>
-      <c r="E174" t="str">
+      <c r="E175" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.mismo.usuario',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'You can´t delete or block yourself')</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>515</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B176" t="s">
         <v>516</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C176" t="s">
         <v>517</v>
       </c>
-      <c r="D175" t="str">
+      <c r="D176" t="str">
         <f t="shared" si="4"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.excedido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'La capacidad del curso fue excedida')</v>
       </c>
-      <c r="E175" t="str">
+      <c r="E176" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.excedido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The course capacity is over the limit')</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>523</v>
+      </c>
+      <c r="B177" t="s">
+        <v>521</v>
+      </c>
+      <c r="C177" t="s">
+        <v>522</v>
+      </c>
+      <c r="D177" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.rango.fecha.invalido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Rango de fechas inválido')</v>
+      </c>
+      <c r="E177" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.rango.fecha.invalido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Invalid Date Range')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-- final fixes  -bitacora rework -promocion de alumnos prevenir la promocion a un nivel sin materias. --close asignacion de materias. --upper case en curso. ---regexs --cambio en la query de niveles para sabes cuales no tienen materias. ..email al usuario en cuenta bloqueada.
</commit_message>
<xml_diff>
--- a/Varios/traducciones.xlsx
+++ b/Varios/traducciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Documents\Trabajo-De-Campo\trabajo-de-diploma\Varios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4A32BC-24C0-47E1-807D-20C1D5776819}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069E7FFA-063C-4A62-8F08-841BE66F2261}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{461B7C5F-BDDA-470F-86DF-9E00192D23ED}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="531">
   <si>
     <t>Alumno</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Familia</t>
   </si>
   <si>
-    <t>Bloqueada</t>
-  </si>
-  <si>
     <t>Patente</t>
   </si>
   <si>
@@ -1604,6 +1601,30 @@
   </si>
   <si>
     <t>com.td.rango.fecha.invalido</t>
+  </si>
+  <si>
+    <t>com.td.email.header.recover</t>
+  </si>
+  <si>
+    <t>com.td.email.body.recover</t>
+  </si>
+  <si>
+    <t>Se detecto actividad sospechosa en su cuenta</t>
+  </si>
+  <si>
+    <t>Por seguridad, se genero esta nueva contraseña:</t>
+  </si>
+  <si>
+    <t>For security, this password was generated:</t>
+  </si>
+  <si>
+    <t>Suspicious activity detected in you account</t>
+  </si>
+  <si>
+    <t>Negada</t>
+  </si>
+  <si>
+    <t>Denied</t>
   </si>
 </sst>
 </file>
@@ -1957,10 +1978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB4AC18-9E40-4F52-A240-1F2EFB37F2BC}">
-  <dimension ref="A1:E177"/>
+  <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E164" workbookViewId="0">
-      <selection activeCell="D177" sqref="D177:E177"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1974,30 +1995,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
       <c r="D1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E1" t="s">
         <v>342</v>
-      </c>
-      <c r="E1" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D65" si="0">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
@@ -2024,13 +2045,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
@@ -2043,13 +2064,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>343</v>
+      </c>
+      <c r="B4" t="s">
         <v>344</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>345</v>
-      </c>
-      <c r="C4" t="s">
-        <v>346</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
@@ -2062,13 +2083,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
@@ -2081,13 +2102,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -2100,13 +2121,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
@@ -2119,13 +2140,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
@@ -2138,13 +2159,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
@@ -2157,13 +2178,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -2176,13 +2197,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
@@ -2195,7 +2216,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -2214,13 +2235,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
@@ -2233,13 +2254,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
@@ -2252,13 +2273,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
@@ -2271,13 +2292,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
@@ -2290,13 +2311,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
@@ -2309,13 +2330,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B18" t="s">
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
@@ -2328,13 +2349,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
@@ -2347,13 +2368,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B20" t="s">
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
@@ -2366,13 +2387,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
@@ -2385,13 +2406,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B22" t="s">
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
@@ -2404,13 +2425,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
@@ -2423,13 +2444,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
@@ -2442,13 +2463,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B25" t="s">
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
@@ -2461,13 +2482,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
@@ -2480,13 +2501,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B27" t="s">
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
@@ -2499,13 +2520,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B28" t="s">
         <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
@@ -2518,13 +2539,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B29" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C29" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
@@ -2537,13 +2558,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B30" t="s">
         <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
@@ -2556,13 +2577,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B31" t="s">
         <v>26</v>
       </c>
       <c r="C31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
@@ -2575,13 +2596,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B32" t="s">
         <v>27</v>
       </c>
       <c r="C32" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
@@ -2594,13 +2615,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B33" t="s">
         <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
@@ -2613,13 +2634,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B34" t="s">
         <v>29</v>
       </c>
       <c r="C34" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
@@ -2632,13 +2653,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B35" t="s">
         <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
@@ -2651,13 +2672,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B36" t="s">
         <v>31</v>
       </c>
       <c r="C36" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
@@ -2670,13 +2691,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B37" t="s">
         <v>32</v>
       </c>
       <c r="C37" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
@@ -2689,13 +2710,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B38" t="s">
         <v>33</v>
       </c>
       <c r="C38" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
@@ -2708,13 +2729,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B39" t="s">
         <v>34</v>
       </c>
       <c r="C39" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
@@ -2727,32 +2748,32 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>529</v>
       </c>
       <c r="C40" t="s">
-        <v>360</v>
+        <v>530</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.bloqueada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Bloqueada')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.bloqueada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Negada')</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="1"/>
-        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.bloqueada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Blocked')</v>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.bloqueada',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Denied')</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C41" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
@@ -2765,13 +2786,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C42" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D42" t="str">
         <f t="shared" si="0"/>
@@ -2784,13 +2805,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C43" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
@@ -2803,13 +2824,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B44" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D44" t="str">
         <f t="shared" si="0"/>
@@ -2822,13 +2843,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="0"/>
@@ -2841,13 +2862,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="0"/>
@@ -2860,13 +2881,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C47" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="0"/>
@@ -2879,13 +2900,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C48" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D48" t="str">
         <f t="shared" si="0"/>
@@ -2898,13 +2919,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C49" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="0"/>
@@ -2917,13 +2938,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C50" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
@@ -2936,13 +2957,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B51" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" si="0"/>
@@ -2955,13 +2976,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>357</v>
+      </c>
+      <c r="B52" t="s">
         <v>358</v>
       </c>
-      <c r="B52" t="s">
-        <v>359</v>
-      </c>
       <c r="C52" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D52" t="str">
         <f t="shared" si="0"/>
@@ -2974,13 +2995,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B53" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C53" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D53" t="str">
         <f t="shared" si="0"/>
@@ -2993,13 +3014,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B54" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C54" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D54" t="str">
         <f t="shared" si="0"/>
@@ -3012,13 +3033,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B55" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C55" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D55" t="str">
         <f t="shared" si="0"/>
@@ -3031,13 +3052,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B56" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C56" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
@@ -3050,13 +3071,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B57" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C57" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D57" t="str">
         <f t="shared" si="0"/>
@@ -3069,13 +3090,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B58" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C58" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D58" t="str">
         <f t="shared" si="0"/>
@@ -3088,13 +3109,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C59" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D59" t="str">
         <f t="shared" si="0"/>
@@ -3107,13 +3128,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C60" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D60" t="str">
         <f t="shared" si="0"/>
@@ -3126,13 +3147,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B61" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C61" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
@@ -3145,13 +3166,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B62" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C62" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
@@ -3164,13 +3185,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C63" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
@@ -3183,13 +3204,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C64" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
@@ -3202,13 +3223,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B65" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C65" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
@@ -3221,13 +3242,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B66" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C66" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D66" t="str">
         <f t="shared" ref="D66:D124" si="2">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
@@ -3254,13 +3275,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C67" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D67" t="str">
         <f t="shared" si="2"/>
@@ -3273,13 +3294,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B68" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C68" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D68" t="str">
         <f t="shared" si="2"/>
@@ -3292,13 +3313,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>517</v>
+      </c>
+      <c r="B69" t="s">
         <v>518</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>519</v>
-      </c>
-      <c r="C69" t="s">
-        <v>520</v>
       </c>
       <c r="D69" t="str">
         <f t="shared" si="2"/>
@@ -3311,13 +3332,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B70" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C70" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="2"/>
@@ -3330,13 +3351,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B71" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C71" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D71" t="str">
         <f t="shared" si="2"/>
@@ -3349,13 +3370,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B72" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C72" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D72" t="str">
         <f t="shared" si="2"/>
@@ -3368,13 +3389,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B73" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C73" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="2"/>
@@ -3387,13 +3408,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B74" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C74" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="2"/>
@@ -3406,13 +3427,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B75" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C75" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="2"/>
@@ -3425,13 +3446,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B76" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C76" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D76" t="str">
         <f t="shared" si="2"/>
@@ -3444,13 +3465,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B77" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="2"/>
@@ -3463,13 +3484,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B78" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C78" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="2"/>
@@ -3482,13 +3503,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B79" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C79" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="2"/>
@@ -3501,13 +3522,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B80" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C80" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D80" t="str">
         <f t="shared" si="2"/>
@@ -3520,13 +3541,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C81" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D81" t="str">
         <f t="shared" si="2"/>
@@ -3539,13 +3560,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B82" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C82" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="2"/>
@@ -3558,13 +3579,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B83" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C83" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D83" t="str">
         <f t="shared" si="2"/>
@@ -3577,13 +3598,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B84" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C84" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D84" t="str">
         <f t="shared" si="2"/>
@@ -3596,13 +3617,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B85" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C85" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D85" t="str">
         <f t="shared" si="2"/>
@@ -3615,13 +3636,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B86" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C86" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D86" t="str">
         <f t="shared" si="2"/>
@@ -3634,13 +3655,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B87" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C87" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D87" t="str">
         <f t="shared" si="2"/>
@@ -3653,13 +3674,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B88" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C88" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D88" t="str">
         <f t="shared" si="2"/>
@@ -3672,13 +3693,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B89" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C89" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D89" t="str">
         <f t="shared" si="2"/>
@@ -3691,13 +3712,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B90" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C90" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D90" t="str">
         <f t="shared" si="2"/>
@@ -3710,13 +3731,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B91" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C91" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D91" t="str">
         <f t="shared" si="2"/>
@@ -3729,13 +3750,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B92" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C92" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D92" t="str">
         <f t="shared" si="2"/>
@@ -3748,13 +3769,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B93" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C93" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D93" t="str">
         <f t="shared" si="2"/>
@@ -3767,13 +3788,13 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B94" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C94" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D94" t="str">
         <f t="shared" si="2"/>
@@ -3786,13 +3807,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B95" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C95" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D95" t="str">
         <f t="shared" si="2"/>
@@ -3805,13 +3826,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B96" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C96" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D96" t="str">
         <f t="shared" si="2"/>
@@ -3824,13 +3845,13 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B97" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C97" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D97" t="str">
         <f t="shared" si="2"/>
@@ -3843,13 +3864,13 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B98" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C98" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D98" t="str">
         <f t="shared" si="2"/>
@@ -3862,13 +3883,13 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B99" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C99" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D99" t="str">
         <f t="shared" si="2"/>
@@ -3881,13 +3902,13 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B100" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C100" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D100" t="str">
         <f t="shared" si="2"/>
@@ -3900,13 +3921,13 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B101" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C101" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D101" t="str">
         <f t="shared" si="2"/>
@@ -3919,13 +3940,13 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B102" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C102" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D102" t="str">
         <f t="shared" si="2"/>
@@ -3938,13 +3959,13 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B103" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C103" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D103" t="str">
         <f t="shared" si="2"/>
@@ -3957,13 +3978,13 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B104" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C104" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D104" t="str">
         <f t="shared" si="2"/>
@@ -3976,13 +3997,13 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B105" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C105" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D105" t="str">
         <f t="shared" si="2"/>
@@ -3995,13 +4016,13 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B106" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C106" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D106" t="str">
         <f t="shared" si="2"/>
@@ -4014,13 +4035,13 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B107" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C107" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D107" t="str">
         <f t="shared" si="2"/>
@@ -4033,13 +4054,13 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B108" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C108" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D108" t="str">
         <f t="shared" si="2"/>
@@ -4052,13 +4073,13 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B109" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C109" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D109" t="str">
         <f t="shared" si="2"/>
@@ -4071,13 +4092,13 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B110" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C110" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D110" t="str">
         <f t="shared" si="2"/>
@@ -4090,13 +4111,13 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B111" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C111" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D111" t="str">
         <f t="shared" si="2"/>
@@ -4109,13 +4130,13 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B112" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C112" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D112" t="str">
         <f t="shared" si="2"/>
@@ -4128,13 +4149,13 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B113" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C113" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D113" t="str">
         <f t="shared" si="2"/>
@@ -4147,13 +4168,13 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B114" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C114" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D114" t="str">
         <f t="shared" si="2"/>
@@ -4166,13 +4187,13 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B115" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C115" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D115" t="str">
         <f t="shared" si="2"/>
@@ -4185,13 +4206,13 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B116" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C116" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D116" t="str">
         <f t="shared" si="2"/>
@@ -4204,13 +4225,13 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B117" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C117" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D117" t="str">
         <f t="shared" si="2"/>
@@ -4223,13 +4244,13 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B118" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C118" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D118" t="str">
         <f t="shared" si="2"/>
@@ -4242,13 +4263,13 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B119" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C119" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D119" t="str">
         <f t="shared" si="2"/>
@@ -4261,13 +4282,13 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B120" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C120" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D120" t="str">
         <f t="shared" si="2"/>
@@ -4280,13 +4301,13 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B121" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C121" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D121" t="str">
         <f t="shared" si="2"/>
@@ -4299,13 +4320,13 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B122" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C122" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D122" t="str">
         <f t="shared" si="2"/>
@@ -4318,13 +4339,13 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
+        <v>346</v>
+      </c>
+      <c r="B123" t="s">
         <v>347</v>
       </c>
-      <c r="B123" t="s">
+      <c r="C123" t="s">
         <v>348</v>
-      </c>
-      <c r="C123" t="s">
-        <v>349</v>
       </c>
       <c r="D123" t="str">
         <f t="shared" si="2"/>
@@ -4337,13 +4358,13 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B124" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C124" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D124" t="str">
         <f t="shared" si="2"/>
@@ -4356,13 +4377,13 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
+        <v>351</v>
+      </c>
+      <c r="B125" t="s">
         <v>352</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C125" t="s">
         <v>353</v>
-      </c>
-      <c r="C125" t="s">
-        <v>354</v>
       </c>
       <c r="D125" t="str">
         <f>CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
@@ -4389,13 +4410,13 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
+        <v>375</v>
+      </c>
+      <c r="B126" t="s">
         <v>376</v>
       </c>
-      <c r="B126" t="s">
+      <c r="C126" t="s">
         <v>377</v>
-      </c>
-      <c r="C126" t="s">
-        <v>378</v>
       </c>
       <c r="D126" t="str">
         <f>CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
@@ -4422,16 +4443,16 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B127" t="s">
         <v>379</v>
       </c>
-      <c r="B127" t="s">
+      <c r="C127" t="s">
         <v>380</v>
       </c>
-      <c r="C127" t="s">
-        <v>381</v>
-      </c>
       <c r="D127" t="str">
-        <f t="shared" ref="D127:D177" si="4">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+        <f t="shared" ref="D127:D179" si="4">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
 values ('",
 $A127,
 "',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
@@ -4442,7 +4463,7 @@
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.motivo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Motivo')</v>
       </c>
       <c r="E127" t="str">
-        <f t="shared" ref="E127:E177" si="5">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+        <f t="shared" ref="E127:E179" si="5">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
 values ('",
 $A127,
 "',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
@@ -4455,13 +4476,13 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
+        <v>381</v>
+      </c>
+      <c r="B128" t="s">
         <v>382</v>
       </c>
-      <c r="B128" t="s">
+      <c r="C128" t="s">
         <v>383</v>
-      </c>
-      <c r="C128" t="s">
-        <v>384</v>
       </c>
       <c r="D128" t="str">
         <f t="shared" si="4"/>
@@ -4474,13 +4495,13 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
+        <v>384</v>
+      </c>
+      <c r="B129" t="s">
+        <v>386</v>
+      </c>
+      <c r="C129" t="s">
         <v>385</v>
-      </c>
-      <c r="B129" t="s">
-        <v>387</v>
-      </c>
-      <c r="C129" t="s">
-        <v>386</v>
       </c>
       <c r="D129" t="str">
         <f t="shared" si="4"/>
@@ -4493,13 +4514,13 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>387</v>
+      </c>
+      <c r="B130" t="s">
         <v>388</v>
       </c>
-      <c r="B130" t="s">
+      <c r="C130" t="s">
         <v>389</v>
-      </c>
-      <c r="C130" t="s">
-        <v>390</v>
       </c>
       <c r="D130" t="str">
         <f t="shared" si="4"/>
@@ -4512,13 +4533,13 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
+        <v>390</v>
+      </c>
+      <c r="B131" t="s">
         <v>391</v>
       </c>
-      <c r="B131" t="s">
+      <c r="C131" t="s">
         <v>392</v>
-      </c>
-      <c r="C131" t="s">
-        <v>393</v>
       </c>
       <c r="D131" t="str">
         <f t="shared" si="4"/>
@@ -4531,13 +4552,13 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B132" t="s">
+        <v>393</v>
+      </c>
+      <c r="C132" t="s">
         <v>394</v>
-      </c>
-      <c r="C132" t="s">
-        <v>395</v>
       </c>
       <c r="D132" t="str">
         <f t="shared" si="4"/>
@@ -4550,13 +4571,13 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B133" t="s">
         <v>396</v>
       </c>
-      <c r="B133" t="s">
-        <v>397</v>
-      </c>
       <c r="C133" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D133" t="str">
         <f t="shared" si="4"/>
@@ -4569,13 +4590,13 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B134" t="s">
         <v>398</v>
       </c>
-      <c r="B134" t="s">
+      <c r="C134" t="s">
         <v>399</v>
-      </c>
-      <c r="C134" t="s">
-        <v>400</v>
       </c>
       <c r="D134" t="str">
         <f t="shared" si="4"/>
@@ -4588,13 +4609,13 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B135" t="s">
         <v>401</v>
       </c>
-      <c r="B135" t="s">
-        <v>402</v>
-      </c>
       <c r="C135" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D135" t="str">
         <f t="shared" si="4"/>
@@ -4607,13 +4628,13 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B136" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C136" t="s">
         <v>404</v>
-      </c>
-      <c r="C136" t="s">
-        <v>405</v>
       </c>
       <c r="D136" t="str">
         <f t="shared" si="4"/>
@@ -4626,13 +4647,13 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="B137" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="C137" t="s">
         <v>408</v>
-      </c>
-      <c r="C137" t="s">
-        <v>409</v>
       </c>
       <c r="D137" t="str">
         <f t="shared" si="4"/>
@@ -4645,13 +4666,13 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C138" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D138" t="str">
         <f t="shared" si="4"/>
@@ -4664,13 +4685,13 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C139" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D139" t="str">
         <f t="shared" si="4"/>
@@ -4683,13 +4704,13 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C140" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D140" t="str">
         <f t="shared" si="4"/>
@@ -4702,13 +4723,13 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B141" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="C141" t="s">
         <v>419</v>
-      </c>
-      <c r="C141" t="s">
-        <v>420</v>
       </c>
       <c r="D141" t="str">
         <f t="shared" si="4"/>
@@ -4721,13 +4742,13 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B142" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C142" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D142" t="str">
         <f t="shared" si="4"/>
@@ -4740,13 +4761,13 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
+        <v>422</v>
+      </c>
+      <c r="B143" t="s">
         <v>423</v>
       </c>
-      <c r="B143" t="s">
+      <c r="C143" t="s">
         <v>424</v>
-      </c>
-      <c r="C143" t="s">
-        <v>425</v>
       </c>
       <c r="D143" t="str">
         <f t="shared" si="4"/>
@@ -4759,13 +4780,13 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>425</v>
+      </c>
+      <c r="B144" t="s">
+        <v>427</v>
+      </c>
+      <c r="C144" t="s">
         <v>426</v>
-      </c>
-      <c r="B144" t="s">
-        <v>428</v>
-      </c>
-      <c r="C144" t="s">
-        <v>427</v>
       </c>
       <c r="D144" t="str">
         <f t="shared" si="4"/>
@@ -4778,13 +4799,13 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
+        <v>428</v>
+      </c>
+      <c r="B145" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="C145" t="s">
         <v>430</v>
-      </c>
-      <c r="C145" t="s">
-        <v>431</v>
       </c>
       <c r="D145" t="str">
         <f t="shared" si="4"/>
@@ -4797,13 +4818,13 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
+        <v>431</v>
+      </c>
+      <c r="B146" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="B146" s="2" t="s">
-        <v>433</v>
-      </c>
       <c r="C146" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D146" t="str">
         <f t="shared" si="4"/>
@@ -4816,13 +4837,13 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
+        <v>433</v>
+      </c>
+      <c r="B147" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="B147" s="2" t="s">
+      <c r="C147" t="s">
         <v>435</v>
-      </c>
-      <c r="C147" t="s">
-        <v>436</v>
       </c>
       <c r="D147" t="str">
         <f t="shared" si="4"/>
@@ -4835,13 +4856,13 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C148" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D148" t="str">
         <f t="shared" si="4"/>
@@ -4854,13 +4875,13 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
+        <v>437</v>
+      </c>
+      <c r="B149" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="B149" s="2" t="s">
+      <c r="C149" t="s">
         <v>439</v>
-      </c>
-      <c r="C149" t="s">
-        <v>440</v>
       </c>
       <c r="D149" t="str">
         <f t="shared" si="4"/>
@@ -4873,13 +4894,13 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
+        <v>440</v>
+      </c>
+      <c r="B150" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="B150" s="2" t="s">
+      <c r="C150" t="s">
         <v>442</v>
-      </c>
-      <c r="C150" t="s">
-        <v>443</v>
       </c>
       <c r="D150" t="str">
         <f t="shared" si="4"/>
@@ -4892,13 +4913,13 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
+        <v>443</v>
+      </c>
+      <c r="B151" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="C151" t="s">
         <v>445</v>
-      </c>
-      <c r="C151" t="s">
-        <v>446</v>
       </c>
       <c r="D151" t="str">
         <f t="shared" si="4"/>
@@ -4911,13 +4932,13 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
+        <v>446</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="C152" t="s">
         <v>448</v>
-      </c>
-      <c r="C152" t="s">
-        <v>449</v>
       </c>
       <c r="D152" t="str">
         <f t="shared" si="4"/>
@@ -4930,13 +4951,13 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
+        <v>449</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="C153" t="s">
         <v>450</v>
-      </c>
-      <c r="B153" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="C153" t="s">
-        <v>451</v>
       </c>
       <c r="D153" t="str">
         <f t="shared" si="4"/>
@@ -4949,13 +4970,13 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
+        <v>452</v>
+      </c>
+      <c r="B154" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="B154" s="2" t="s">
+      <c r="C154" t="s">
         <v>454</v>
-      </c>
-      <c r="C154" t="s">
-        <v>455</v>
       </c>
       <c r="D154" t="str">
         <f t="shared" si="4"/>
@@ -4968,13 +4989,13 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
+        <v>455</v>
+      </c>
+      <c r="B155" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="C155" t="s">
         <v>457</v>
-      </c>
-      <c r="C155" t="s">
-        <v>458</v>
       </c>
       <c r="D155" t="str">
         <f t="shared" si="4"/>
@@ -4987,13 +5008,13 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
+        <v>459</v>
+      </c>
+      <c r="B156" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="B156" s="2" t="s">
+      <c r="C156" t="s">
         <v>461</v>
-      </c>
-      <c r="C156" t="s">
-        <v>462</v>
       </c>
       <c r="D156" t="str">
         <f t="shared" si="4"/>
@@ -5006,13 +5027,13 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
+        <v>462</v>
+      </c>
+      <c r="B157" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="B157" s="2" t="s">
+      <c r="C157" t="s">
         <v>464</v>
-      </c>
-      <c r="C157" t="s">
-        <v>465</v>
       </c>
       <c r="D157" t="str">
         <f t="shared" si="4"/>
@@ -5025,13 +5046,13 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>465</v>
+      </c>
+      <c r="B158" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="B158" s="2" t="s">
+      <c r="C158" t="s">
         <v>467</v>
-      </c>
-      <c r="C158" t="s">
-        <v>468</v>
       </c>
       <c r="D158" t="str">
         <f t="shared" si="4"/>
@@ -5044,13 +5065,13 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
+        <v>468</v>
+      </c>
+      <c r="B159" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="B159" s="2" t="s">
+      <c r="C159" t="s">
         <v>470</v>
-      </c>
-      <c r="C159" t="s">
-        <v>471</v>
       </c>
       <c r="D159" t="str">
         <f t="shared" si="4"/>
@@ -5063,13 +5084,13 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
+        <v>471</v>
+      </c>
+      <c r="B160" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="B160" s="2" t="s">
+      <c r="C160" t="s">
         <v>473</v>
-      </c>
-      <c r="C160" t="s">
-        <v>474</v>
       </c>
       <c r="D160" t="str">
         <f t="shared" si="4"/>
@@ -5082,13 +5103,13 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
+        <v>474</v>
+      </c>
+      <c r="B161" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="B161" s="2" t="s">
+      <c r="C161" t="s">
         <v>476</v>
-      </c>
-      <c r="C161" t="s">
-        <v>477</v>
       </c>
       <c r="D161" t="str">
         <f t="shared" si="4"/>
@@ -5101,13 +5122,13 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
+        <v>477</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="C162" t="s">
         <v>478</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="C162" t="s">
-        <v>479</v>
       </c>
       <c r="D162" t="str">
         <f t="shared" si="4"/>
@@ -5120,13 +5141,13 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
+        <v>480</v>
+      </c>
+      <c r="B163" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="B163" s="2" t="s">
+      <c r="C163" t="s">
         <v>482</v>
-      </c>
-      <c r="C163" t="s">
-        <v>483</v>
       </c>
       <c r="D163" t="str">
         <f t="shared" si="4"/>
@@ -5139,13 +5160,13 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
+        <v>483</v>
+      </c>
+      <c r="B164" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="B164" s="2" t="s">
+      <c r="C164" t="s">
         <v>485</v>
-      </c>
-      <c r="C164" t="s">
-        <v>486</v>
       </c>
       <c r="D164" t="str">
         <f t="shared" si="4"/>
@@ -5158,13 +5179,13 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
+        <v>486</v>
+      </c>
+      <c r="B165" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="B165" s="2" t="s">
+      <c r="C165" t="s">
         <v>488</v>
-      </c>
-      <c r="C165" t="s">
-        <v>489</v>
       </c>
       <c r="D165" t="str">
         <f t="shared" si="4"/>
@@ -5177,13 +5198,13 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B166" t="s">
         <v>361</v>
       </c>
-      <c r="B166" t="s">
+      <c r="C166" t="s">
         <v>362</v>
-      </c>
-      <c r="C166" t="s">
-        <v>363</v>
       </c>
       <c r="D166" t="str">
         <f t="shared" si="4"/>
@@ -5196,13 +5217,13 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
+        <v>363</v>
+      </c>
+      <c r="B167" t="s">
         <v>364</v>
       </c>
-      <c r="B167" t="s">
+      <c r="C167" t="s">
         <v>365</v>
-      </c>
-      <c r="C167" t="s">
-        <v>366</v>
       </c>
       <c r="D167" t="str">
         <f t="shared" si="4"/>
@@ -5215,13 +5236,13 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
+        <v>490</v>
+      </c>
+      <c r="B168" t="s">
         <v>491</v>
       </c>
-      <c r="B168" t="s">
+      <c r="C168" t="s">
         <v>492</v>
-      </c>
-      <c r="C168" t="s">
-        <v>493</v>
       </c>
       <c r="D168" t="str">
         <f t="shared" si="4"/>
@@ -5234,13 +5255,13 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
+        <v>493</v>
+      </c>
+      <c r="B169" t="s">
         <v>494</v>
       </c>
-      <c r="B169" t="s">
+      <c r="C169" t="s">
         <v>495</v>
-      </c>
-      <c r="C169" t="s">
-        <v>496</v>
       </c>
       <c r="D169" t="str">
         <f t="shared" si="4"/>
@@ -5253,13 +5274,13 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
+        <v>496</v>
+      </c>
+      <c r="B170" t="s">
         <v>497</v>
       </c>
-      <c r="B170" t="s">
+      <c r="C170" t="s">
         <v>498</v>
-      </c>
-      <c r="C170" t="s">
-        <v>499</v>
       </c>
       <c r="D170" t="str">
         <f t="shared" si="4"/>
@@ -5272,13 +5293,13 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
+        <v>499</v>
+      </c>
+      <c r="B171" t="s">
         <v>500</v>
       </c>
-      <c r="B171" t="s">
+      <c r="C171" t="s">
         <v>501</v>
-      </c>
-      <c r="C171" t="s">
-        <v>502</v>
       </c>
       <c r="D171" t="str">
         <f t="shared" si="4"/>
@@ -5291,13 +5312,13 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
+        <v>502</v>
+      </c>
+      <c r="B172" t="s">
         <v>503</v>
       </c>
-      <c r="B172" t="s">
+      <c r="C172" t="s">
         <v>504</v>
-      </c>
-      <c r="C172" t="s">
-        <v>505</v>
       </c>
       <c r="D172" t="str">
         <f t="shared" si="4"/>
@@ -5310,13 +5331,13 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
+        <v>505</v>
+      </c>
+      <c r="B173" t="s">
         <v>506</v>
       </c>
-      <c r="B173" t="s">
+      <c r="C173" t="s">
         <v>507</v>
-      </c>
-      <c r="C173" t="s">
-        <v>508</v>
       </c>
       <c r="D173" t="str">
         <f t="shared" si="4"/>
@@ -5329,13 +5350,13 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
+        <v>508</v>
+      </c>
+      <c r="B174" t="s">
         <v>509</v>
       </c>
-      <c r="B174" t="s">
+      <c r="C174" t="s">
         <v>510</v>
-      </c>
-      <c r="C174" t="s">
-        <v>511</v>
       </c>
       <c r="D174" t="str">
         <f t="shared" si="4"/>
@@ -5348,13 +5369,13 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
+        <v>511</v>
+      </c>
+      <c r="B175" t="s">
         <v>512</v>
       </c>
-      <c r="B175" t="s">
+      <c r="C175" t="s">
         <v>513</v>
-      </c>
-      <c r="C175" t="s">
-        <v>514</v>
       </c>
       <c r="D175" t="str">
         <f t="shared" si="4"/>
@@ -5367,13 +5388,13 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
+        <v>514</v>
+      </c>
+      <c r="B176" t="s">
         <v>515</v>
       </c>
-      <c r="B176" t="s">
+      <c r="C176" t="s">
         <v>516</v>
-      </c>
-      <c r="C176" t="s">
-        <v>517</v>
       </c>
       <c r="D176" t="str">
         <f t="shared" si="4"/>
@@ -5386,13 +5407,13 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B177" t="s">
+        <v>520</v>
+      </c>
+      <c r="C177" t="s">
         <v>521</v>
-      </c>
-      <c r="C177" t="s">
-        <v>522</v>
       </c>
       <c r="D177" t="str">
         <f t="shared" si="4"/>
@@ -5401,6 +5422,44 @@
       <c r="E177" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.rango.fecha.invalido',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Invalid Date Range')</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="B178" t="s">
+        <v>525</v>
+      </c>
+      <c r="C178" t="s">
+        <v>528</v>
+      </c>
+      <c r="D178" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.header.recover',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Se detecto actividad sospechosa en su cuenta')</v>
+      </c>
+      <c r="E178" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.header.recover',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'Suspicious activity detected in you account')</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>524</v>
+      </c>
+      <c r="B179" t="s">
+        <v>526</v>
+      </c>
+      <c r="C179" t="s">
+        <v>527</v>
+      </c>
+      <c r="D179" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.body.recover',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Por seguridad, se genero esta nueva contraseña:')</v>
+      </c>
+      <c r="E179" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.body.recover',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'For security, this password was generated:')</v>
       </c>
     </row>
   </sheetData>
@@ -5428,30 +5487,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
       <c r="D1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E1" t="s">
         <v>342</v>
-      </c>
-      <c r="E1" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C2" t="s">
         <v>373</v>
-      </c>
-      <c r="C2" t="s">
-        <v>374</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D7" si="0">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
@@ -5478,13 +5537,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>355</v>
+      </c>
+      <c r="B3" t="s">
         <v>356</v>
       </c>
-      <c r="B3" t="s">
-        <v>357</v>
-      </c>
       <c r="C3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
@@ -5497,13 +5556,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>360</v>
+      </c>
+      <c r="B4" t="s">
         <v>361</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>362</v>
-      </c>
-      <c r="C4" t="s">
-        <v>363</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
@@ -5516,13 +5575,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>363</v>
+      </c>
+      <c r="B5" t="s">
         <v>364</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>365</v>
-      </c>
-      <c r="C5" t="s">
-        <v>366</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
@@ -5535,13 +5594,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>366</v>
+      </c>
+      <c r="B6" t="s">
         <v>367</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>368</v>
-      </c>
-      <c r="C6" t="s">
-        <v>369</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -5554,13 +5613,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>369</v>
+      </c>
+      <c r="B7" t="s">
         <v>370</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>371</v>
-      </c>
-      <c r="C7" t="s">
-        <v>372</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
--hago el chequeo de que la contraseña sea igual a la que esta estoreada antes de actualizar
</commit_message>
<xml_diff>
--- a/Varios/traducciones.xlsx
+++ b/Varios/traducciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Documents\Trabajo-De-Campo\trabajo-de-diploma\Varios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Documents\TrabajoDeCampo\trabajo-de-diploma\Varios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069E7FFA-063C-4A62-8F08-841BE66F2261}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77268CF8-A361-4653-B3B0-A35214B21422}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{461B7C5F-BDDA-470F-86DF-9E00192D23ED}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Controles" sheetId="1" r:id="rId1"/>
     <sheet name="Mensajes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="534">
   <si>
     <t>Alumno</t>
   </si>
@@ -1625,6 +1624,15 @@
   </si>
   <si>
     <t>Denied</t>
+  </si>
+  <si>
+    <t>com.td.contraseña.distinta</t>
+  </si>
+  <si>
+    <t>La contraseña ingresada como actual es incorrecta</t>
+  </si>
+  <si>
+    <t>The pass entered as actual is incorrect</t>
   </si>
 </sst>
 </file>
@@ -1978,10 +1986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB4AC18-9E40-4F52-A240-1F2EFB37F2BC}">
-  <dimension ref="A1:E179"/>
+  <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="A180" sqref="A180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4452,7 +4460,7 @@
         <v>380</v>
       </c>
       <c r="D127" t="str">
-        <f t="shared" ref="D127:D179" si="4">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+        <f t="shared" ref="D127:D180" si="4">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
 values ('",
 $A127,
 "',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
@@ -4463,7 +4471,7 @@
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.motivo',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'Motivo')</v>
       </c>
       <c r="E127" t="str">
-        <f t="shared" ref="E127:E179" si="5">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
+        <f t="shared" ref="E127:E180" si="5">CLEAN(_xlfn.CONCAT("insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)
 values ('",
 $A127,
 "',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = '",
@@ -5460,6 +5468,25 @@
       <c r="E179" t="str">
         <f t="shared" si="5"/>
         <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.email.body.recover',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'For security, this password was generated:')</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>531</v>
+      </c>
+      <c r="B180" t="s">
+        <v>532</v>
+      </c>
+      <c r="C180" t="s">
+        <v>533</v>
+      </c>
+      <c r="D180" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.contraseña.distinta',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'es'),'La contraseña ingresada como actual es incorrecta')</v>
+      </c>
+      <c r="E180" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into MENSAJE(MSJ_CODIGO,MSJ_IDIOMA_ID,MSJ_TEXTO)values ('com.td.contraseña.distinta',( select idioma.IDI_ID from IDIOMA where IDI_CODIGO = 'en'),'The pass entered as actual is incorrect')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>